<commit_message>
reporting model minor fixes
</commit_message>
<xml_diff>
--- a/ADSDataDirect.Web/Templates/ReTargeting.xlsx
+++ b/ADSDataDirect.Web/Templates/ReTargeting.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="36">
   <si>
     <t>URLS</t>
   </si>
@@ -33,9 +33,6 @@
     <t>Link</t>
   </si>
   <si>
-    <t>Delivered</t>
-  </si>
-  <si>
     <t xml:space="preserve">Kia of Tallahasse </t>
   </si>
   <si>
@@ -67,9 +64,6 @@
   </si>
   <si>
     <t xml:space="preserve"> Send Performance</t>
-  </si>
-  <si>
-    <t>Delivery Rate</t>
   </si>
   <si>
     <t>Deployed</t>
@@ -924,17 +918,44 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="34" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="26" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="5" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1" indent="5"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1" indent="5"/>
+    </xf>
     <xf numFmtId="0" fontId="27" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1" indent="5"/>
     </xf>
     <xf numFmtId="0" fontId="27" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1" indent="5"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="5" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1" indent="5"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1" indent="5"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="27" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1" indent="5"/>
@@ -942,6 +963,18 @@
     <xf numFmtId="0" fontId="27" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1" indent="5"/>
     </xf>
+    <xf numFmtId="0" fontId="25" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="5" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1" indent="5"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1" indent="5"/>
+    </xf>
     <xf numFmtId="0" fontId="27" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1" indent="5"/>
     </xf>
@@ -950,45 +983,6 @@
     </xf>
     <xf numFmtId="0" fontId="27" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1" indent="5"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="5" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1" indent="5"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1" indent="5"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1057,7 +1051,7 @@
         <xdr:cNvPr id="8" name="Picture 7">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6DEF1A45-3E5D-462A-91AF-E22A9FC6595F}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{6DEF1A45-3E5D-462A-91AF-E22A9FC6595F}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1069,7 +1063,7 @@
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" val="0"/>
+              <a14:useLocalDpi xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
@@ -1107,7 +1101,7 @@
         <xdr:cNvPr id="9" name="Picture 8">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E5E130FC-7FBD-4FEF-956C-6BF505EDB0A7}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{E5E130FC-7FBD-4FEF-956C-6BF505EDB0A7}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1119,7 +1113,7 @@
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" val="0"/>
+              <a14:useLocalDpi xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
@@ -1157,7 +1151,7 @@
         <xdr:cNvPr id="10" name="Picture 9">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5D019ABE-D70D-4CF3-99C2-0C11B1E847CC}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{5D019ABE-D70D-4CF3-99C2-0C11B1E847CC}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1169,7 +1163,7 @@
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" val="0"/>
+              <a14:useLocalDpi xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
@@ -1202,7 +1196,7 @@
         <xdr:cNvPr id="11" name="Picture 10" descr="Image result for retargeting image icons transparent gif">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0800-00000E000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0800-00000E000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1214,7 +1208,7 @@
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
@@ -1234,7 +1228,7 @@
         <a:noFill/>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
@@ -1537,7 +1531,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1550,8 +1544,8 @@
   </sheetPr>
   <dimension ref="A1:J117"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
-      <selection activeCell="C45" sqref="C45"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8:J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -1638,37 +1632,37 @@
       <c r="G6" s="57"/>
       <c r="I6" s="7"/>
       <c r="J6" s="76" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" s="16" customFormat="1" ht="21.9" customHeight="1">
+      <c r="A7" s="80" t="s">
+        <v>27</v>
+      </c>
+      <c r="B7" s="80"/>
+      <c r="C7" s="80"/>
+      <c r="D7" s="80"/>
+      <c r="E7" s="80"/>
+      <c r="F7" s="80"/>
+      <c r="G7" s="80"/>
+      <c r="H7" s="80"/>
+      <c r="I7" s="80"/>
+      <c r="J7" s="80"/>
+    </row>
+    <row r="8" spans="1:10" ht="26.25" customHeight="1">
+      <c r="A8" s="89" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="7" spans="1:10" s="16" customFormat="1" ht="21.9" customHeight="1">
-      <c r="A7" s="98" t="s">
-        <v>29</v>
-      </c>
-      <c r="B7" s="98"/>
-      <c r="C7" s="98"/>
-      <c r="D7" s="98"/>
-      <c r="E7" s="98"/>
-      <c r="F7" s="98"/>
-      <c r="G7" s="98"/>
-      <c r="H7" s="98"/>
-      <c r="I7" s="98"/>
-      <c r="J7" s="98"/>
-    </row>
-    <row r="8" spans="1:10" ht="26.25" customHeight="1">
-      <c r="A8" s="93" t="s">
+      <c r="B8" s="91" t="s">
+        <v>4</v>
+      </c>
+      <c r="C8" s="91"/>
+      <c r="D8" s="91"/>
+      <c r="E8" s="91"/>
+      <c r="F8" s="91"/>
+      <c r="G8" s="91"/>
+      <c r="H8" s="49" t="s">
         <v>11</v>
-      </c>
-      <c r="B8" s="95" t="s">
-        <v>5</v>
-      </c>
-      <c r="C8" s="95"/>
-      <c r="D8" s="95"/>
-      <c r="E8" s="95"/>
-      <c r="F8" s="95"/>
-      <c r="G8" s="95"/>
-      <c r="H8" s="49" t="s">
-        <v>12</v>
       </c>
       <c r="I8" s="50"/>
       <c r="J8" s="51">
@@ -1676,15 +1670,15 @@
       </c>
     </row>
     <row r="9" spans="1:10" ht="26.25" customHeight="1">
-      <c r="A9" s="94"/>
-      <c r="B9" s="96"/>
-      <c r="C9" s="96"/>
-      <c r="D9" s="96"/>
-      <c r="E9" s="96"/>
-      <c r="F9" s="96"/>
-      <c r="G9" s="96"/>
+      <c r="A9" s="90"/>
+      <c r="B9" s="92"/>
+      <c r="C9" s="92"/>
+      <c r="D9" s="92"/>
+      <c r="E9" s="92"/>
+      <c r="F9" s="92"/>
+      <c r="G9" s="92"/>
       <c r="H9" s="49" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I9" s="50"/>
       <c r="J9" s="52">
@@ -1692,15 +1686,15 @@
       </c>
     </row>
     <row r="10" spans="1:10" ht="26.25" customHeight="1">
-      <c r="A10" s="94"/>
-      <c r="B10" s="96"/>
-      <c r="C10" s="96"/>
-      <c r="D10" s="96"/>
-      <c r="E10" s="96"/>
-      <c r="F10" s="96"/>
-      <c r="G10" s="96"/>
+      <c r="A10" s="90"/>
+      <c r="B10" s="92"/>
+      <c r="C10" s="92"/>
+      <c r="D10" s="92"/>
+      <c r="E10" s="92"/>
+      <c r="F10" s="92"/>
+      <c r="G10" s="92"/>
       <c r="H10" s="49" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="I10" s="50"/>
       <c r="J10" s="52">
@@ -1708,18 +1702,18 @@
       </c>
     </row>
     <row r="11" spans="1:10" ht="25.8">
-      <c r="A11" s="100" t="s">
-        <v>31</v>
-      </c>
-      <c r="B11" s="101"/>
-      <c r="C11" s="101"/>
-      <c r="D11" s="101"/>
-      <c r="E11" s="101"/>
-      <c r="F11" s="101"/>
-      <c r="G11" s="101"/>
-      <c r="H11" s="101"/>
-      <c r="I11" s="101"/>
-      <c r="J11" s="101"/>
+      <c r="A11" s="83" t="s">
+        <v>29</v>
+      </c>
+      <c r="B11" s="84"/>
+      <c r="C11" s="84"/>
+      <c r="D11" s="84"/>
+      <c r="E11" s="84"/>
+      <c r="F11" s="84"/>
+      <c r="G11" s="84"/>
+      <c r="H11" s="84"/>
+      <c r="I11" s="84"/>
+      <c r="J11" s="84"/>
     </row>
     <row r="12" spans="1:10" ht="20.100000000000001" customHeight="1">
       <c r="A12" s="1"/>
@@ -1735,14 +1729,14 @@
     </row>
     <row r="13" spans="1:10" ht="35.1" customHeight="1">
       <c r="A13" s="48" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B13" s="19"/>
       <c r="C13" s="53"/>
       <c r="D13" s="53"/>
       <c r="E13" s="3"/>
       <c r="F13" s="45" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="G13" s="34"/>
       <c r="H13" s="34"/>
@@ -1751,20 +1745,16 @@
     </row>
     <row r="14" spans="1:10" ht="17.399999999999999">
       <c r="A14" s="20"/>
-      <c r="B14" s="21" t="s">
-        <v>16</v>
-      </c>
-      <c r="C14" s="22">
-        <v>0.98360000000000003</v>
-      </c>
+      <c r="B14" s="21"/>
+      <c r="C14" s="22"/>
       <c r="D14" s="22"/>
       <c r="E14" s="3"/>
       <c r="F14" s="35" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G14" s="36"/>
       <c r="H14" s="37" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="I14" s="38"/>
       <c r="J14" s="46"/>
@@ -1772,7 +1762,7 @@
     <row r="15" spans="1:10" ht="15.75" customHeight="1">
       <c r="A15" s="20"/>
       <c r="B15" s="21" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C15" s="23">
         <v>100000</v>
@@ -1780,23 +1770,19 @@
       <c r="D15" s="23"/>
       <c r="E15" s="3"/>
       <c r="F15" s="39" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G15" s="23"/>
       <c r="H15" s="40" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="I15" s="41"/>
       <c r="J15" s="46"/>
     </row>
     <row r="16" spans="1:10" ht="15.75" customHeight="1">
       <c r="A16" s="24"/>
-      <c r="B16" s="25" t="s">
-        <v>4</v>
-      </c>
-      <c r="C16" s="23">
-        <v>98360</v>
-      </c>
+      <c r="B16" s="25"/>
+      <c r="C16" s="23"/>
       <c r="D16" s="23"/>
       <c r="E16" s="3"/>
       <c r="F16" s="19"/>
@@ -1806,8 +1792,8 @@
       <c r="J16" s="19"/>
     </row>
     <row r="17" spans="1:10" ht="15.6">
-      <c r="A17" s="99"/>
-      <c r="B17" s="99"/>
+      <c r="A17" s="82"/>
+      <c r="B17" s="82"/>
       <c r="C17" s="19"/>
       <c r="D17" s="19"/>
       <c r="E17" s="3"/>
@@ -1818,8 +1804,8 @@
       <c r="J17" s="19"/>
     </row>
     <row r="18" spans="1:10" ht="15.75" customHeight="1">
-      <c r="A18" s="99"/>
-      <c r="B18" s="99"/>
+      <c r="A18" s="82"/>
+      <c r="B18" s="82"/>
       <c r="C18" s="19"/>
       <c r="D18" s="19"/>
       <c r="E18" s="3"/>
@@ -1843,7 +1829,7 @@
     </row>
     <row r="20" spans="1:10" ht="31.2">
       <c r="A20" s="45" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B20" s="26"/>
       <c r="C20" s="19"/>
@@ -1870,7 +1856,7 @@
     <row r="22" spans="1:10" ht="31.2">
       <c r="A22" s="19"/>
       <c r="B22" s="27" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C22" s="28">
         <v>0.17513000000000001</v>
@@ -1886,7 +1872,7 @@
     <row r="23" spans="1:10" ht="31.2">
       <c r="A23" s="19"/>
       <c r="B23" s="21" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C23" s="23">
         <v>17513</v>
@@ -1943,13 +1929,13 @@
     </row>
     <row r="27" spans="1:10">
       <c r="A27" s="31" t="s">
+        <v>19</v>
+      </c>
+      <c r="B27" s="31" t="s">
+        <v>20</v>
+      </c>
+      <c r="C27" s="31" t="s">
         <v>21</v>
-      </c>
-      <c r="B27" s="31" t="s">
-        <v>22</v>
-      </c>
-      <c r="C27" s="31" t="s">
-        <v>23</v>
       </c>
       <c r="D27" s="31"/>
       <c r="E27" s="3"/>
@@ -1989,10 +1975,10 @@
     </row>
     <row r="30" spans="1:10" ht="20.100000000000001" customHeight="1">
       <c r="A30" s="56" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B30" s="56" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C30" s="56"/>
       <c r="D30" s="56"/>
@@ -2040,8 +2026,8 @@
       <c r="J33" s="19"/>
     </row>
     <row r="34" spans="1:10" ht="15.6">
-      <c r="A34" s="97" t="s">
-        <v>24</v>
+      <c r="A34" s="81" t="s">
+        <v>22</v>
       </c>
       <c r="B34" s="26"/>
       <c r="C34" s="19"/>
@@ -2054,7 +2040,7 @@
       <c r="J34" s="19"/>
     </row>
     <row r="35" spans="1:10">
-      <c r="A35" s="97"/>
+      <c r="A35" s="81"/>
       <c r="B35" s="19"/>
       <c r="C35" s="19"/>
       <c r="D35" s="19"/>
@@ -2080,7 +2066,7 @@
     <row r="37" spans="1:10" ht="21">
       <c r="A37" s="19"/>
       <c r="B37" s="27" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C37" s="32">
         <v>1340</v>
@@ -2096,7 +2082,7 @@
     <row r="38" spans="1:10" ht="21">
       <c r="A38" s="19"/>
       <c r="B38" s="27" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C38" s="33">
         <v>1279</v>
@@ -2134,8 +2120,8 @@
       <c r="J40" s="19"/>
     </row>
     <row r="41" spans="1:10" ht="15.6" customHeight="1">
-      <c r="A41" s="97" t="s">
-        <v>35</v>
+      <c r="A41" s="81" t="s">
+        <v>33</v>
       </c>
       <c r="B41" s="19"/>
       <c r="C41" s="19"/>
@@ -2148,7 +2134,7 @@
       <c r="J41" s="19"/>
     </row>
     <row r="42" spans="1:10" ht="14.4" customHeight="1">
-      <c r="A42" s="97"/>
+      <c r="A42" s="81"/>
       <c r="B42" s="19"/>
       <c r="C42" s="19"/>
       <c r="D42" s="19"/>
@@ -2174,7 +2160,7 @@
     <row r="44" spans="1:10" ht="18">
       <c r="A44" s="19"/>
       <c r="B44" s="77" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C44" s="78">
         <v>972</v>
@@ -2190,7 +2176,7 @@
     <row r="45" spans="1:10" ht="18">
       <c r="A45" s="19"/>
       <c r="B45" s="79" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C45" s="78">
         <v>972</v>
@@ -2265,7 +2251,7 @@
     </row>
     <row r="51" spans="1:10">
       <c r="A51" s="58" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B51" s="9"/>
       <c r="C51" s="9"/>
@@ -2526,23 +2512,23 @@
       <c r="F72" s="7"/>
       <c r="I72" s="7"/>
       <c r="J72" s="76" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="73" spans="1:10" ht="21">
+      <c r="A73" s="89" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="73" spans="1:10" ht="21">
-      <c r="A73" s="93" t="s">
+      <c r="B73" s="91" t="s">
+        <v>4</v>
+      </c>
+      <c r="C73" s="91"/>
+      <c r="D73" s="91"/>
+      <c r="E73" s="91"/>
+      <c r="F73" s="91"/>
+      <c r="G73" s="91"/>
+      <c r="H73" s="49" t="s">
         <v>11</v>
-      </c>
-      <c r="B73" s="95" t="s">
-        <v>5</v>
-      </c>
-      <c r="C73" s="95"/>
-      <c r="D73" s="95"/>
-      <c r="E73" s="95"/>
-      <c r="F73" s="95"/>
-      <c r="G73" s="95"/>
-      <c r="H73" s="49" t="s">
-        <v>12</v>
       </c>
       <c r="I73" s="50"/>
       <c r="J73" s="51">
@@ -2550,15 +2536,15 @@
       </c>
     </row>
     <row r="74" spans="1:10" ht="21">
-      <c r="A74" s="94"/>
-      <c r="B74" s="96"/>
-      <c r="C74" s="96"/>
-      <c r="D74" s="96"/>
-      <c r="E74" s="96"/>
-      <c r="F74" s="96"/>
-      <c r="G74" s="96"/>
+      <c r="A74" s="90"/>
+      <c r="B74" s="92"/>
+      <c r="C74" s="92"/>
+      <c r="D74" s="92"/>
+      <c r="E74" s="92"/>
+      <c r="F74" s="92"/>
+      <c r="G74" s="92"/>
       <c r="H74" s="49" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I74" s="50"/>
       <c r="J74" s="52">
@@ -2566,15 +2552,15 @@
       </c>
     </row>
     <row r="75" spans="1:10" ht="21">
-      <c r="A75" s="94"/>
-      <c r="B75" s="96"/>
-      <c r="C75" s="96"/>
-      <c r="D75" s="96"/>
-      <c r="E75" s="96"/>
-      <c r="F75" s="96"/>
-      <c r="G75" s="96"/>
+      <c r="A75" s="90"/>
+      <c r="B75" s="92"/>
+      <c r="C75" s="92"/>
+      <c r="D75" s="92"/>
+      <c r="E75" s="92"/>
+      <c r="F75" s="92"/>
+      <c r="G75" s="92"/>
       <c r="H75" s="49" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="I75" s="50"/>
       <c r="J75" s="52">
@@ -2595,7 +2581,7 @@
     </row>
     <row r="77" spans="1:10" ht="15" customHeight="1">
       <c r="A77" s="10" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B77" s="11"/>
       <c r="C77" s="11"/>
@@ -2632,15 +2618,15 @@
       <c r="J79" s="8"/>
     </row>
     <row r="80" spans="1:10" ht="23.4">
-      <c r="A80" s="91" t="s">
+      <c r="A80" s="95" t="s">
         <v>0</v>
       </c>
-      <c r="B80" s="91"/>
-      <c r="C80" s="91"/>
-      <c r="D80" s="91"/>
-      <c r="E80" s="92"/>
+      <c r="B80" s="95"/>
+      <c r="C80" s="95"/>
+      <c r="D80" s="95"/>
+      <c r="E80" s="96"/>
       <c r="F80" s="66" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="G80" s="67" t="s">
         <v>1</v>
@@ -2666,524 +2652,529 @@
       <c r="J81" s="63"/>
     </row>
     <row r="82" spans="1:10" ht="50.1" customHeight="1">
-      <c r="A82" s="89"/>
-      <c r="B82" s="90"/>
-      <c r="C82" s="90"/>
-      <c r="D82" s="90"/>
-      <c r="E82" s="90"/>
+      <c r="A82" s="97"/>
+      <c r="B82" s="98"/>
+      <c r="C82" s="98"/>
+      <c r="D82" s="98"/>
+      <c r="E82" s="98"/>
       <c r="F82" s="68"/>
       <c r="G82" s="68"/>
       <c r="H82" s="68"/>
       <c r="I82" s="69" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="J82" s="3"/>
     </row>
     <row r="83" spans="1:10" ht="50.1" customHeight="1">
-      <c r="A83" s="80"/>
-      <c r="B83" s="81"/>
-      <c r="C83" s="81"/>
-      <c r="D83" s="81"/>
-      <c r="E83" s="81"/>
+      <c r="A83" s="87"/>
+      <c r="B83" s="88"/>
+      <c r="C83" s="88"/>
+      <c r="D83" s="88"/>
+      <c r="E83" s="88"/>
       <c r="F83" s="61"/>
       <c r="G83" s="61"/>
       <c r="H83" s="61"/>
       <c r="I83" s="70" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="J83" s="3"/>
     </row>
     <row r="84" spans="1:10" ht="50.1" customHeight="1">
-      <c r="A84" s="82"/>
-      <c r="B84" s="83"/>
-      <c r="C84" s="83"/>
-      <c r="D84" s="83"/>
-      <c r="E84" s="83"/>
+      <c r="A84" s="85"/>
+      <c r="B84" s="86"/>
+      <c r="C84" s="86"/>
+      <c r="D84" s="86"/>
+      <c r="E84" s="86"/>
       <c r="F84" s="60"/>
       <c r="G84" s="60"/>
       <c r="H84" s="60"/>
       <c r="I84" s="71" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="J84" s="3"/>
     </row>
     <row r="85" spans="1:10" ht="50.1" customHeight="1">
-      <c r="A85" s="80"/>
-      <c r="B85" s="81"/>
-      <c r="C85" s="81"/>
-      <c r="D85" s="81"/>
-      <c r="E85" s="81"/>
+      <c r="A85" s="87"/>
+      <c r="B85" s="88"/>
+      <c r="C85" s="88"/>
+      <c r="D85" s="88"/>
+      <c r="E85" s="88"/>
       <c r="F85" s="61"/>
       <c r="G85" s="61"/>
       <c r="H85" s="61"/>
       <c r="I85" s="70" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="J85" s="3"/>
     </row>
     <row r="86" spans="1:10" ht="50.1" customHeight="1">
-      <c r="A86" s="82"/>
-      <c r="B86" s="83"/>
-      <c r="C86" s="83"/>
-      <c r="D86" s="83"/>
-      <c r="E86" s="83"/>
+      <c r="A86" s="85"/>
+      <c r="B86" s="86"/>
+      <c r="C86" s="86"/>
+      <c r="D86" s="86"/>
+      <c r="E86" s="86"/>
       <c r="F86" s="60"/>
       <c r="G86" s="60"/>
       <c r="H86" s="60"/>
       <c r="I86" s="71" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="J86" s="3"/>
     </row>
     <row r="87" spans="1:10" ht="50.1" customHeight="1">
-      <c r="A87" s="80"/>
-      <c r="B87" s="81"/>
-      <c r="C87" s="81"/>
-      <c r="D87" s="81"/>
-      <c r="E87" s="81"/>
+      <c r="A87" s="87"/>
+      <c r="B87" s="88"/>
+      <c r="C87" s="88"/>
+      <c r="D87" s="88"/>
+      <c r="E87" s="88"/>
       <c r="F87" s="61"/>
       <c r="G87" s="61"/>
       <c r="H87" s="61"/>
       <c r="I87" s="70" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="J87" s="3"/>
     </row>
     <row r="88" spans="1:10" ht="50.1" customHeight="1">
-      <c r="A88" s="82"/>
-      <c r="B88" s="83"/>
-      <c r="C88" s="83"/>
-      <c r="D88" s="83"/>
-      <c r="E88" s="83"/>
+      <c r="A88" s="85"/>
+      <c r="B88" s="86"/>
+      <c r="C88" s="86"/>
+      <c r="D88" s="86"/>
+      <c r="E88" s="86"/>
       <c r="F88" s="60"/>
       <c r="G88" s="60"/>
       <c r="H88" s="60"/>
       <c r="I88" s="71" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="J88" s="3"/>
     </row>
     <row r="89" spans="1:10" ht="50.1" customHeight="1">
-      <c r="A89" s="80"/>
-      <c r="B89" s="81"/>
-      <c r="C89" s="81"/>
-      <c r="D89" s="81"/>
-      <c r="E89" s="81"/>
+      <c r="A89" s="87"/>
+      <c r="B89" s="88"/>
+      <c r="C89" s="88"/>
+      <c r="D89" s="88"/>
+      <c r="E89" s="88"/>
       <c r="F89" s="61"/>
       <c r="G89" s="61"/>
       <c r="H89" s="61"/>
       <c r="I89" s="70" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="J89" s="3"/>
     </row>
     <row r="90" spans="1:10" ht="50.1" customHeight="1">
-      <c r="A90" s="82"/>
-      <c r="B90" s="83"/>
-      <c r="C90" s="83"/>
-      <c r="D90" s="83"/>
-      <c r="E90" s="83"/>
+      <c r="A90" s="85"/>
+      <c r="B90" s="86"/>
+      <c r="C90" s="86"/>
+      <c r="D90" s="86"/>
+      <c r="E90" s="86"/>
       <c r="F90" s="60"/>
       <c r="G90" s="60"/>
       <c r="H90" s="60"/>
       <c r="I90" s="71" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="J90" s="3"/>
     </row>
     <row r="91" spans="1:10" ht="50.1" customHeight="1">
-      <c r="A91" s="80"/>
-      <c r="B91" s="81"/>
-      <c r="C91" s="81"/>
-      <c r="D91" s="81"/>
-      <c r="E91" s="81"/>
+      <c r="A91" s="87"/>
+      <c r="B91" s="88"/>
+      <c r="C91" s="88"/>
+      <c r="D91" s="88"/>
+      <c r="E91" s="88"/>
       <c r="F91" s="61"/>
       <c r="G91" s="61"/>
       <c r="H91" s="61"/>
       <c r="I91" s="70" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="J91" s="3"/>
     </row>
     <row r="92" spans="1:10" ht="50.1" customHeight="1">
-      <c r="A92" s="82"/>
-      <c r="B92" s="83"/>
-      <c r="C92" s="83"/>
-      <c r="D92" s="83"/>
-      <c r="E92" s="83"/>
+      <c r="A92" s="85"/>
+      <c r="B92" s="86"/>
+      <c r="C92" s="86"/>
+      <c r="D92" s="86"/>
+      <c r="E92" s="86"/>
       <c r="F92" s="60"/>
       <c r="G92" s="60"/>
       <c r="H92" s="60"/>
       <c r="I92" s="72" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="J92" s="3"/>
     </row>
     <row r="93" spans="1:10" ht="50.1" customHeight="1">
-      <c r="A93" s="80"/>
-      <c r="B93" s="81"/>
-      <c r="C93" s="81"/>
-      <c r="D93" s="81"/>
-      <c r="E93" s="81"/>
+      <c r="A93" s="87"/>
+      <c r="B93" s="88"/>
+      <c r="C93" s="88"/>
+      <c r="D93" s="88"/>
+      <c r="E93" s="88"/>
       <c r="F93" s="61"/>
       <c r="G93" s="61"/>
       <c r="H93" s="61"/>
       <c r="I93" s="73" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="J93" s="3"/>
     </row>
     <row r="94" spans="1:10" ht="50.1" customHeight="1">
-      <c r="A94" s="82"/>
-      <c r="B94" s="83"/>
-      <c r="C94" s="83"/>
-      <c r="D94" s="83"/>
-      <c r="E94" s="83"/>
+      <c r="A94" s="85"/>
+      <c r="B94" s="86"/>
+      <c r="C94" s="86"/>
+      <c r="D94" s="86"/>
+      <c r="E94" s="86"/>
       <c r="F94" s="60"/>
       <c r="G94" s="60"/>
       <c r="H94" s="60"/>
       <c r="I94" s="71" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="J94" s="3"/>
     </row>
     <row r="95" spans="1:10" ht="50.1" customHeight="1">
-      <c r="A95" s="86"/>
-      <c r="B95" s="87"/>
-      <c r="C95" s="87"/>
-      <c r="D95" s="87"/>
-      <c r="E95" s="88"/>
+      <c r="A95" s="99"/>
+      <c r="B95" s="100"/>
+      <c r="C95" s="100"/>
+      <c r="D95" s="100"/>
+      <c r="E95" s="101"/>
       <c r="F95" s="61"/>
       <c r="G95" s="61"/>
       <c r="H95" s="61"/>
       <c r="I95" s="70" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="J95" s="3"/>
     </row>
     <row r="96" spans="1:10" ht="50.1" customHeight="1">
-      <c r="A96" s="82"/>
-      <c r="B96" s="83"/>
-      <c r="C96" s="83"/>
-      <c r="D96" s="83"/>
-      <c r="E96" s="83"/>
+      <c r="A96" s="85"/>
+      <c r="B96" s="86"/>
+      <c r="C96" s="86"/>
+      <c r="D96" s="86"/>
+      <c r="E96" s="86"/>
       <c r="F96" s="60"/>
       <c r="G96" s="60"/>
       <c r="H96" s="60"/>
       <c r="I96" s="71" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="J96" s="3"/>
     </row>
     <row r="97" spans="1:10" ht="50.1" customHeight="1">
-      <c r="A97" s="80"/>
-      <c r="B97" s="81"/>
-      <c r="C97" s="81"/>
-      <c r="D97" s="81"/>
-      <c r="E97" s="81"/>
+      <c r="A97" s="87"/>
+      <c r="B97" s="88"/>
+      <c r="C97" s="88"/>
+      <c r="D97" s="88"/>
+      <c r="E97" s="88"/>
       <c r="F97" s="61"/>
       <c r="G97" s="61"/>
       <c r="H97" s="61"/>
       <c r="I97" s="70" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="J97" s="3"/>
     </row>
     <row r="98" spans="1:10" ht="50.1" customHeight="1">
-      <c r="A98" s="82"/>
-      <c r="B98" s="83"/>
-      <c r="C98" s="83"/>
-      <c r="D98" s="83"/>
-      <c r="E98" s="83"/>
+      <c r="A98" s="85"/>
+      <c r="B98" s="86"/>
+      <c r="C98" s="86"/>
+      <c r="D98" s="86"/>
+      <c r="E98" s="86"/>
       <c r="F98" s="60"/>
       <c r="G98" s="60"/>
       <c r="H98" s="60"/>
       <c r="I98" s="72" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="J98" s="3"/>
     </row>
     <row r="99" spans="1:10" ht="50.1" customHeight="1">
-      <c r="A99" s="84"/>
-      <c r="B99" s="85"/>
-      <c r="C99" s="85"/>
-      <c r="D99" s="85"/>
-      <c r="E99" s="85"/>
+      <c r="A99" s="93"/>
+      <c r="B99" s="94"/>
+      <c r="C99" s="94"/>
+      <c r="D99" s="94"/>
+      <c r="E99" s="94"/>
       <c r="F99" s="74"/>
       <c r="G99" s="74"/>
       <c r="H99" s="74"/>
       <c r="I99" s="75" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="J99" s="3"/>
     </row>
     <row r="100" spans="1:10" ht="50.1" customHeight="1">
-      <c r="A100" s="89"/>
-      <c r="B100" s="90"/>
-      <c r="C100" s="90"/>
-      <c r="D100" s="90"/>
-      <c r="E100" s="90"/>
+      <c r="A100" s="97"/>
+      <c r="B100" s="98"/>
+      <c r="C100" s="98"/>
+      <c r="D100" s="98"/>
+      <c r="E100" s="98"/>
       <c r="F100" s="68"/>
       <c r="G100" s="68"/>
       <c r="H100" s="68"/>
       <c r="I100" s="69" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="J100" s="3"/>
     </row>
     <row r="101" spans="1:10" ht="50.1" customHeight="1">
-      <c r="A101" s="80"/>
-      <c r="B101" s="81"/>
-      <c r="C101" s="81"/>
-      <c r="D101" s="81"/>
-      <c r="E101" s="81"/>
+      <c r="A101" s="87"/>
+      <c r="B101" s="88"/>
+      <c r="C101" s="88"/>
+      <c r="D101" s="88"/>
+      <c r="E101" s="88"/>
       <c r="F101" s="61"/>
       <c r="G101" s="61"/>
       <c r="H101" s="61"/>
       <c r="I101" s="70" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="J101" s="3"/>
     </row>
     <row r="102" spans="1:10" ht="50.1" customHeight="1">
-      <c r="A102" s="82"/>
-      <c r="B102" s="83"/>
-      <c r="C102" s="83"/>
-      <c r="D102" s="83"/>
-      <c r="E102" s="83"/>
+      <c r="A102" s="85"/>
+      <c r="B102" s="86"/>
+      <c r="C102" s="86"/>
+      <c r="D102" s="86"/>
+      <c r="E102" s="86"/>
       <c r="F102" s="60"/>
       <c r="G102" s="60"/>
       <c r="H102" s="60"/>
       <c r="I102" s="71" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="J102" s="3"/>
     </row>
     <row r="103" spans="1:10" ht="50.1" customHeight="1">
-      <c r="A103" s="80"/>
-      <c r="B103" s="81"/>
-      <c r="C103" s="81"/>
-      <c r="D103" s="81"/>
-      <c r="E103" s="81"/>
+      <c r="A103" s="87"/>
+      <c r="B103" s="88"/>
+      <c r="C103" s="88"/>
+      <c r="D103" s="88"/>
+      <c r="E103" s="88"/>
       <c r="F103" s="61"/>
       <c r="G103" s="61"/>
       <c r="H103" s="61"/>
       <c r="I103" s="70" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="J103" s="3"/>
     </row>
     <row r="104" spans="1:10" ht="50.1" customHeight="1">
-      <c r="A104" s="82"/>
-      <c r="B104" s="83"/>
-      <c r="C104" s="83"/>
-      <c r="D104" s="83"/>
-      <c r="E104" s="83"/>
+      <c r="A104" s="85"/>
+      <c r="B104" s="86"/>
+      <c r="C104" s="86"/>
+      <c r="D104" s="86"/>
+      <c r="E104" s="86"/>
       <c r="F104" s="60"/>
       <c r="G104" s="60"/>
       <c r="H104" s="60"/>
       <c r="I104" s="71" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="J104" s="3"/>
     </row>
     <row r="105" spans="1:10" ht="50.1" customHeight="1">
-      <c r="A105" s="80"/>
-      <c r="B105" s="81"/>
-      <c r="C105" s="81"/>
-      <c r="D105" s="81"/>
-      <c r="E105" s="81"/>
+      <c r="A105" s="87"/>
+      <c r="B105" s="88"/>
+      <c r="C105" s="88"/>
+      <c r="D105" s="88"/>
+      <c r="E105" s="88"/>
       <c r="F105" s="61"/>
       <c r="G105" s="61"/>
       <c r="H105" s="61"/>
       <c r="I105" s="70" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="J105" s="3"/>
     </row>
     <row r="106" spans="1:10" ht="50.1" customHeight="1">
-      <c r="A106" s="82"/>
-      <c r="B106" s="83"/>
-      <c r="C106" s="83"/>
-      <c r="D106" s="83"/>
-      <c r="E106" s="83"/>
+      <c r="A106" s="85"/>
+      <c r="B106" s="86"/>
+      <c r="C106" s="86"/>
+      <c r="D106" s="86"/>
+      <c r="E106" s="86"/>
       <c r="F106" s="60"/>
       <c r="G106" s="60"/>
       <c r="H106" s="60"/>
       <c r="I106" s="71" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="J106" s="3"/>
     </row>
     <row r="107" spans="1:10" ht="50.1" customHeight="1">
-      <c r="A107" s="80"/>
-      <c r="B107" s="81"/>
-      <c r="C107" s="81"/>
-      <c r="D107" s="81"/>
-      <c r="E107" s="81"/>
+      <c r="A107" s="87"/>
+      <c r="B107" s="88"/>
+      <c r="C107" s="88"/>
+      <c r="D107" s="88"/>
+      <c r="E107" s="88"/>
       <c r="F107" s="61"/>
       <c r="G107" s="61"/>
       <c r="H107" s="61"/>
       <c r="I107" s="70" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="J107" s="3"/>
     </row>
     <row r="108" spans="1:10" ht="50.1" customHeight="1">
-      <c r="A108" s="82"/>
-      <c r="B108" s="83"/>
-      <c r="C108" s="83"/>
-      <c r="D108" s="83"/>
-      <c r="E108" s="83"/>
+      <c r="A108" s="85"/>
+      <c r="B108" s="86"/>
+      <c r="C108" s="86"/>
+      <c r="D108" s="86"/>
+      <c r="E108" s="86"/>
       <c r="F108" s="60"/>
       <c r="G108" s="60"/>
       <c r="H108" s="60"/>
       <c r="I108" s="71" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="J108" s="3"/>
     </row>
     <row r="109" spans="1:10" ht="50.1" customHeight="1">
-      <c r="A109" s="80"/>
-      <c r="B109" s="81"/>
-      <c r="C109" s="81"/>
-      <c r="D109" s="81"/>
-      <c r="E109" s="81"/>
+      <c r="A109" s="87"/>
+      <c r="B109" s="88"/>
+      <c r="C109" s="88"/>
+      <c r="D109" s="88"/>
+      <c r="E109" s="88"/>
       <c r="F109" s="61"/>
       <c r="G109" s="61"/>
       <c r="H109" s="61"/>
       <c r="I109" s="70" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="J109" s="3"/>
     </row>
     <row r="110" spans="1:10" ht="50.1" customHeight="1">
-      <c r="A110" s="82"/>
-      <c r="B110" s="83"/>
-      <c r="C110" s="83"/>
-      <c r="D110" s="83"/>
-      <c r="E110" s="83"/>
+      <c r="A110" s="85"/>
+      <c r="B110" s="86"/>
+      <c r="C110" s="86"/>
+      <c r="D110" s="86"/>
+      <c r="E110" s="86"/>
       <c r="F110" s="60"/>
       <c r="G110" s="60"/>
       <c r="H110" s="60"/>
       <c r="I110" s="72" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="J110" s="3"/>
     </row>
     <row r="111" spans="1:10" ht="50.1" customHeight="1">
-      <c r="A111" s="80"/>
-      <c r="B111" s="81"/>
-      <c r="C111" s="81"/>
-      <c r="D111" s="81"/>
-      <c r="E111" s="81"/>
+      <c r="A111" s="87"/>
+      <c r="B111" s="88"/>
+      <c r="C111" s="88"/>
+      <c r="D111" s="88"/>
+      <c r="E111" s="88"/>
       <c r="F111" s="61"/>
       <c r="G111" s="61"/>
       <c r="H111" s="61"/>
       <c r="I111" s="73" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="J111" s="3"/>
     </row>
     <row r="112" spans="1:10" ht="50.1" customHeight="1">
-      <c r="A112" s="82"/>
-      <c r="B112" s="83"/>
-      <c r="C112" s="83"/>
-      <c r="D112" s="83"/>
-      <c r="E112" s="83"/>
+      <c r="A112" s="85"/>
+      <c r="B112" s="86"/>
+      <c r="C112" s="86"/>
+      <c r="D112" s="86"/>
+      <c r="E112" s="86"/>
       <c r="F112" s="60"/>
       <c r="G112" s="60"/>
       <c r="H112" s="60"/>
       <c r="I112" s="71" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="J112" s="3"/>
     </row>
     <row r="113" spans="1:10" ht="50.1" customHeight="1">
-      <c r="A113" s="86"/>
-      <c r="B113" s="87"/>
-      <c r="C113" s="87"/>
-      <c r="D113" s="87"/>
-      <c r="E113" s="88"/>
+      <c r="A113" s="99"/>
+      <c r="B113" s="100"/>
+      <c r="C113" s="100"/>
+      <c r="D113" s="100"/>
+      <c r="E113" s="101"/>
       <c r="F113" s="61"/>
       <c r="G113" s="61"/>
       <c r="H113" s="61"/>
       <c r="I113" s="70" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="J113" s="3"/>
     </row>
     <row r="114" spans="1:10" ht="50.1" customHeight="1">
-      <c r="A114" s="82"/>
-      <c r="B114" s="83"/>
-      <c r="C114" s="83"/>
-      <c r="D114" s="83"/>
-      <c r="E114" s="83"/>
+      <c r="A114" s="85"/>
+      <c r="B114" s="86"/>
+      <c r="C114" s="86"/>
+      <c r="D114" s="86"/>
+      <c r="E114" s="86"/>
       <c r="F114" s="60"/>
       <c r="G114" s="60"/>
       <c r="H114" s="60"/>
       <c r="I114" s="71" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="J114" s="3"/>
     </row>
     <row r="115" spans="1:10" ht="50.1" customHeight="1">
-      <c r="A115" s="80"/>
-      <c r="B115" s="81"/>
-      <c r="C115" s="81"/>
-      <c r="D115" s="81"/>
-      <c r="E115" s="81"/>
+      <c r="A115" s="87"/>
+      <c r="B115" s="88"/>
+      <c r="C115" s="88"/>
+      <c r="D115" s="88"/>
+      <c r="E115" s="88"/>
       <c r="F115" s="61"/>
       <c r="G115" s="61"/>
       <c r="H115" s="61"/>
       <c r="I115" s="70" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="J115" s="3"/>
     </row>
     <row r="116" spans="1:10" ht="50.1" customHeight="1">
-      <c r="A116" s="82"/>
-      <c r="B116" s="83"/>
-      <c r="C116" s="83"/>
-      <c r="D116" s="83"/>
-      <c r="E116" s="83"/>
+      <c r="A116" s="85"/>
+      <c r="B116" s="86"/>
+      <c r="C116" s="86"/>
+      <c r="D116" s="86"/>
+      <c r="E116" s="86"/>
       <c r="F116" s="60"/>
       <c r="G116" s="60"/>
       <c r="H116" s="60"/>
       <c r="I116" s="72" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="J116" s="3"/>
     </row>
     <row r="117" spans="1:10" ht="50.1" customHeight="1">
-      <c r="A117" s="84"/>
-      <c r="B117" s="85"/>
-      <c r="C117" s="85"/>
-      <c r="D117" s="85"/>
-      <c r="E117" s="85"/>
+      <c r="A117" s="93"/>
+      <c r="B117" s="94"/>
+      <c r="C117" s="94"/>
+      <c r="D117" s="94"/>
+      <c r="E117" s="94"/>
       <c r="F117" s="74"/>
       <c r="G117" s="74"/>
       <c r="H117" s="74"/>
       <c r="I117" s="75" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="J117" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="47">
-    <mergeCell ref="A7:J7"/>
-    <mergeCell ref="A34:A35"/>
-    <mergeCell ref="A17:B17"/>
-    <mergeCell ref="A18:B18"/>
-    <mergeCell ref="A11:J11"/>
-    <mergeCell ref="A84:E84"/>
-    <mergeCell ref="A85:E85"/>
-    <mergeCell ref="A86:E86"/>
-    <mergeCell ref="A8:A10"/>
-    <mergeCell ref="B8:G10"/>
-    <mergeCell ref="A73:A75"/>
-    <mergeCell ref="B73:G75"/>
-    <mergeCell ref="A41:A42"/>
+    <mergeCell ref="A115:E115"/>
+    <mergeCell ref="A116:E116"/>
+    <mergeCell ref="A117:E117"/>
+    <mergeCell ref="A110:E110"/>
+    <mergeCell ref="A111:E111"/>
+    <mergeCell ref="A112:E112"/>
+    <mergeCell ref="A113:E113"/>
+    <mergeCell ref="A114:E114"/>
+    <mergeCell ref="A105:E105"/>
+    <mergeCell ref="A106:E106"/>
+    <mergeCell ref="A107:E107"/>
+    <mergeCell ref="A108:E108"/>
+    <mergeCell ref="A109:E109"/>
+    <mergeCell ref="A100:E100"/>
+    <mergeCell ref="A101:E101"/>
+    <mergeCell ref="A102:E102"/>
+    <mergeCell ref="A103:E103"/>
+    <mergeCell ref="A104:E104"/>
     <mergeCell ref="A97:E97"/>
     <mergeCell ref="A98:E98"/>
     <mergeCell ref="A99:E99"/>
@@ -3200,24 +3191,19 @@
     <mergeCell ref="A90:E90"/>
     <mergeCell ref="A91:E91"/>
     <mergeCell ref="A95:E95"/>
-    <mergeCell ref="A100:E100"/>
-    <mergeCell ref="A101:E101"/>
-    <mergeCell ref="A102:E102"/>
-    <mergeCell ref="A103:E103"/>
-    <mergeCell ref="A104:E104"/>
-    <mergeCell ref="A105:E105"/>
-    <mergeCell ref="A106:E106"/>
-    <mergeCell ref="A107:E107"/>
-    <mergeCell ref="A108:E108"/>
-    <mergeCell ref="A109:E109"/>
-    <mergeCell ref="A115:E115"/>
-    <mergeCell ref="A116:E116"/>
-    <mergeCell ref="A117:E117"/>
-    <mergeCell ref="A110:E110"/>
-    <mergeCell ref="A111:E111"/>
-    <mergeCell ref="A112:E112"/>
-    <mergeCell ref="A113:E113"/>
-    <mergeCell ref="A114:E114"/>
+    <mergeCell ref="A84:E84"/>
+    <mergeCell ref="A85:E85"/>
+    <mergeCell ref="A86:E86"/>
+    <mergeCell ref="A8:A10"/>
+    <mergeCell ref="B8:G10"/>
+    <mergeCell ref="A73:A75"/>
+    <mergeCell ref="B73:G75"/>
+    <mergeCell ref="A41:A42"/>
+    <mergeCell ref="A7:J7"/>
+    <mergeCell ref="A34:A35"/>
+    <mergeCell ref="A17:B17"/>
+    <mergeCell ref="A18:B18"/>
+    <mergeCell ref="A11:J11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="57" fitToHeight="0" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>

</xml_diff>

<commit_message>
fixed template reports, added opener layout
</commit_message>
<xml_diff>
--- a/ADSDataDirect.Web/Templates/ReTargeting.xlsx
+++ b/ADSDataDirect.Web/Templates/ReTargeting.xlsx
@@ -133,9 +133,8 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+  <numFmts count="1">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="35">
     <font>
@@ -741,7 +740,7 @@
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="102">
+  <cellXfs count="105">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -793,9 +792,6 @@
     </xf>
     <xf numFmtId="0" fontId="20" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="10" fontId="7" fillId="5" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="16" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="10" fontId="16" fillId="5" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -914,16 +910,64 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="32" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="164" fontId="33" fillId="5" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="34" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="27" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1" indent="5"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1" indent="5"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="5" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1" indent="5"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1" indent="5"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1" indent="5"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1" indent="5"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1" indent="5"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1" indent="5"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1" indent="5"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="5" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1" indent="5"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1" indent="5"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="26" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="17" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -933,56 +977,14 @@
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="5" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1" indent="5"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1" indent="5"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1" indent="5"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1" indent="5"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1" indent="5"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1" indent="5"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="5" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1" indent="5"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1" indent="5"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1" indent="5"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1" indent="5"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1" indent="5"/>
+    <xf numFmtId="37" fontId="15" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="37" fontId="16" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="37" fontId="22" fillId="5" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="37" fontId="22" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="37" fontId="33" fillId="5" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1051,7 +1053,7 @@
         <xdr:cNvPr id="8" name="Picture 7">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{6DEF1A45-3E5D-462A-91AF-E22A9FC6595F}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6DEF1A45-3E5D-462A-91AF-E22A9FC6595F}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1063,7 +1065,7 @@
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
@@ -1101,7 +1103,7 @@
         <xdr:cNvPr id="9" name="Picture 8">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{E5E130FC-7FBD-4FEF-956C-6BF505EDB0A7}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E5E130FC-7FBD-4FEF-956C-6BF505EDB0A7}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1113,7 +1115,7 @@
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
@@ -1151,7 +1153,7 @@
         <xdr:cNvPr id="10" name="Picture 9">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{5D019ABE-D70D-4CF3-99C2-0C11B1E847CC}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5D019ABE-D70D-4CF3-99C2-0C11B1E847CC}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1163,7 +1165,7 @@
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
@@ -1196,7 +1198,7 @@
         <xdr:cNvPr id="11" name="Picture 10" descr="Image result for retargeting image icons transparent gif">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0800-00000E000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0800-00000E000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1208,7 +1210,7 @@
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" val="0"/>
+              <a14:useLocalDpi xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
@@ -1228,7 +1230,7 @@
         <a:noFill/>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
+            <a14:hiddenFill xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
@@ -1531,7 +1533,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1629,91 +1631,91 @@
       <c r="D6" s="7"/>
       <c r="E6" s="7"/>
       <c r="F6" s="7"/>
-      <c r="G6" s="57"/>
+      <c r="G6" s="56"/>
       <c r="I6" s="7"/>
-      <c r="J6" s="76" t="s">
+      <c r="J6" s="75" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="7" spans="1:10" s="16" customFormat="1" ht="21.9" customHeight="1">
-      <c r="A7" s="80" t="s">
+      <c r="A7" s="96" t="s">
         <v>27</v>
       </c>
-      <c r="B7" s="80"/>
-      <c r="C7" s="80"/>
-      <c r="D7" s="80"/>
-      <c r="E7" s="80"/>
-      <c r="F7" s="80"/>
-      <c r="G7" s="80"/>
-      <c r="H7" s="80"/>
-      <c r="I7" s="80"/>
-      <c r="J7" s="80"/>
+      <c r="B7" s="96"/>
+      <c r="C7" s="96"/>
+      <c r="D7" s="96"/>
+      <c r="E7" s="96"/>
+      <c r="F7" s="96"/>
+      <c r="G7" s="96"/>
+      <c r="H7" s="96"/>
+      <c r="I7" s="96"/>
+      <c r="J7" s="96"/>
     </row>
     <row r="8" spans="1:10" ht="26.25" customHeight="1">
-      <c r="A8" s="89" t="s">
+      <c r="A8" s="91" t="s">
         <v>10</v>
       </c>
-      <c r="B8" s="91" t="s">
+      <c r="B8" s="93" t="s">
         <v>4</v>
       </c>
-      <c r="C8" s="91"/>
-      <c r="D8" s="91"/>
-      <c r="E8" s="91"/>
-      <c r="F8" s="91"/>
-      <c r="G8" s="91"/>
-      <c r="H8" s="49" t="s">
+      <c r="C8" s="93"/>
+      <c r="D8" s="93"/>
+      <c r="E8" s="93"/>
+      <c r="F8" s="93"/>
+      <c r="G8" s="93"/>
+      <c r="H8" s="48" t="s">
         <v>11</v>
       </c>
-      <c r="I8" s="50"/>
-      <c r="J8" s="51">
+      <c r="I8" s="49"/>
+      <c r="J8" s="50">
         <v>2665</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="26.25" customHeight="1">
-      <c r="A9" s="90"/>
-      <c r="B9" s="92"/>
-      <c r="C9" s="92"/>
-      <c r="D9" s="92"/>
-      <c r="E9" s="92"/>
-      <c r="F9" s="92"/>
-      <c r="G9" s="92"/>
-      <c r="H9" s="49" t="s">
+      <c r="A9" s="92"/>
+      <c r="B9" s="94"/>
+      <c r="C9" s="94"/>
+      <c r="D9" s="94"/>
+      <c r="E9" s="94"/>
+      <c r="F9" s="94"/>
+      <c r="G9" s="94"/>
+      <c r="H9" s="48" t="s">
         <v>12</v>
       </c>
-      <c r="I9" s="50"/>
-      <c r="J9" s="52">
+      <c r="I9" s="49"/>
+      <c r="J9" s="51">
         <v>42901</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="26.25" customHeight="1">
-      <c r="A10" s="90"/>
-      <c r="B10" s="92"/>
-      <c r="C10" s="92"/>
-      <c r="D10" s="92"/>
-      <c r="E10" s="92"/>
-      <c r="F10" s="92"/>
-      <c r="G10" s="92"/>
-      <c r="H10" s="49" t="s">
+      <c r="A10" s="92"/>
+      <c r="B10" s="94"/>
+      <c r="C10" s="94"/>
+      <c r="D10" s="94"/>
+      <c r="E10" s="94"/>
+      <c r="F10" s="94"/>
+      <c r="G10" s="94"/>
+      <c r="H10" s="48" t="s">
         <v>5</v>
       </c>
-      <c r="I10" s="50"/>
-      <c r="J10" s="52">
+      <c r="I10" s="49"/>
+      <c r="J10" s="51">
         <v>42901</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="25.8">
-      <c r="A11" s="83" t="s">
+      <c r="A11" s="98" t="s">
         <v>29</v>
       </c>
-      <c r="B11" s="84"/>
-      <c r="C11" s="84"/>
-      <c r="D11" s="84"/>
-      <c r="E11" s="84"/>
-      <c r="F11" s="84"/>
-      <c r="G11" s="84"/>
-      <c r="H11" s="84"/>
-      <c r="I11" s="84"/>
-      <c r="J11" s="84"/>
+      <c r="B11" s="99"/>
+      <c r="C11" s="99"/>
+      <c r="D11" s="99"/>
+      <c r="E11" s="99"/>
+      <c r="F11" s="99"/>
+      <c r="G11" s="99"/>
+      <c r="H11" s="99"/>
+      <c r="I11" s="99"/>
+      <c r="J11" s="99"/>
     </row>
     <row r="12" spans="1:10" ht="20.100000000000001" customHeight="1">
       <c r="A12" s="1"/>
@@ -1728,20 +1730,20 @@
       <c r="J12" s="1"/>
     </row>
     <row r="13" spans="1:10" ht="35.1" customHeight="1">
-      <c r="A13" s="48" t="s">
+      <c r="A13" s="47" t="s">
         <v>14</v>
       </c>
       <c r="B13" s="19"/>
-      <c r="C13" s="53"/>
-      <c r="D13" s="53"/>
+      <c r="C13" s="52"/>
+      <c r="D13" s="52"/>
       <c r="E13" s="3"/>
-      <c r="F13" s="45" t="s">
+      <c r="F13" s="44" t="s">
         <v>28</v>
       </c>
-      <c r="G13" s="34"/>
-      <c r="H13" s="34"/>
-      <c r="I13" s="34"/>
-      <c r="J13" s="34"/>
+      <c r="G13" s="33"/>
+      <c r="H13" s="33"/>
+      <c r="I13" s="33"/>
+      <c r="J13" s="33"/>
     </row>
     <row r="14" spans="1:10" ht="17.399999999999999">
       <c r="A14" s="20"/>
@@ -1749,35 +1751,35 @@
       <c r="C14" s="22"/>
       <c r="D14" s="22"/>
       <c r="E14" s="3"/>
-      <c r="F14" s="35" t="s">
+      <c r="F14" s="34" t="s">
         <v>13</v>
       </c>
-      <c r="G14" s="36"/>
-      <c r="H14" s="37" t="s">
+      <c r="G14" s="35"/>
+      <c r="H14" s="36" t="s">
         <v>8</v>
       </c>
-      <c r="I14" s="38"/>
-      <c r="J14" s="46"/>
+      <c r="I14" s="37"/>
+      <c r="J14" s="45"/>
     </row>
     <row r="15" spans="1:10" ht="15.75" customHeight="1">
       <c r="A15" s="20"/>
       <c r="B15" s="21" t="s">
         <v>15</v>
       </c>
-      <c r="C15" s="23">
+      <c r="C15" s="100">
         <v>100000</v>
       </c>
       <c r="D15" s="23"/>
       <c r="E15" s="3"/>
-      <c r="F15" s="39" t="s">
+      <c r="F15" s="38" t="s">
         <v>6</v>
       </c>
       <c r="G15" s="23"/>
-      <c r="H15" s="40" t="s">
+      <c r="H15" s="39" t="s">
         <v>7</v>
       </c>
-      <c r="I15" s="41"/>
-      <c r="J15" s="46"/>
+      <c r="I15" s="40"/>
+      <c r="J15" s="45"/>
     </row>
     <row r="16" spans="1:10" ht="15.75" customHeight="1">
       <c r="A16" s="24"/>
@@ -1792,8 +1794,8 @@
       <c r="J16" s="19"/>
     </row>
     <row r="17" spans="1:10" ht="15.6">
-      <c r="A17" s="82"/>
-      <c r="B17" s="82"/>
+      <c r="A17" s="97"/>
+      <c r="B17" s="97"/>
       <c r="C17" s="19"/>
       <c r="D17" s="19"/>
       <c r="E17" s="3"/>
@@ -1804,16 +1806,16 @@
       <c r="J17" s="19"/>
     </row>
     <row r="18" spans="1:10" ht="15.75" customHeight="1">
-      <c r="A18" s="82"/>
-      <c r="B18" s="82"/>
+      <c r="A18" s="97"/>
+      <c r="B18" s="97"/>
       <c r="C18" s="19"/>
       <c r="D18" s="19"/>
       <c r="E18" s="3"/>
-      <c r="F18" s="42"/>
-      <c r="G18" s="42"/>
-      <c r="H18" s="47"/>
+      <c r="F18" s="41"/>
+      <c r="G18" s="41"/>
+      <c r="H18" s="46"/>
       <c r="I18" s="19"/>
-      <c r="J18" s="44"/>
+      <c r="J18" s="43"/>
     </row>
     <row r="19" spans="1:10" ht="24.9" customHeight="1">
       <c r="A19" s="18"/>
@@ -1821,31 +1823,31 @@
       <c r="C19" s="17"/>
       <c r="D19" s="17"/>
       <c r="E19" s="3"/>
-      <c r="F19" s="42"/>
-      <c r="G19" s="42"/>
-      <c r="H19" s="47"/>
+      <c r="F19" s="41"/>
+      <c r="G19" s="41"/>
+      <c r="H19" s="46"/>
       <c r="I19" s="19"/>
-      <c r="J19" s="44"/>
+      <c r="J19" s="43"/>
     </row>
     <row r="20" spans="1:10" ht="31.2">
-      <c r="A20" s="45" t="s">
+      <c r="A20" s="44" t="s">
         <v>16</v>
       </c>
       <c r="B20" s="26"/>
       <c r="C20" s="19"/>
       <c r="D20" s="19"/>
       <c r="E20" s="3"/>
-      <c r="F20" s="42"/>
-      <c r="G20" s="42"/>
-      <c r="H20" s="43"/>
+      <c r="F20" s="41"/>
+      <c r="G20" s="41"/>
+      <c r="H20" s="42"/>
       <c r="I20" s="19"/>
-      <c r="J20" s="44"/>
+      <c r="J20" s="43"/>
     </row>
     <row r="21" spans="1:10" ht="31.2">
       <c r="A21" s="19"/>
       <c r="B21" s="19"/>
-      <c r="C21" s="53"/>
-      <c r="D21" s="53"/>
+      <c r="C21" s="52"/>
+      <c r="D21" s="52"/>
       <c r="E21" s="3"/>
       <c r="F21" s="19"/>
       <c r="G21" s="19"/>
@@ -1863,27 +1865,27 @@
       </c>
       <c r="D22" s="28"/>
       <c r="E22" s="3"/>
-      <c r="F22" s="42"/>
-      <c r="G22" s="42"/>
-      <c r="H22" s="43"/>
+      <c r="F22" s="41"/>
+      <c r="G22" s="41"/>
+      <c r="H22" s="42"/>
       <c r="I22" s="19"/>
-      <c r="J22" s="44"/>
+      <c r="J22" s="43"/>
     </row>
     <row r="23" spans="1:10" ht="31.2">
       <c r="A23" s="19"/>
       <c r="B23" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="C23" s="23">
+      <c r="C23" s="100">
         <v>17513</v>
       </c>
       <c r="D23" s="23"/>
       <c r="E23" s="3"/>
       <c r="F23" s="19"/>
       <c r="G23" s="19"/>
-      <c r="H23" s="43"/>
+      <c r="H23" s="42"/>
       <c r="I23" s="19"/>
-      <c r="J23" s="44"/>
+      <c r="J23" s="43"/>
     </row>
     <row r="24" spans="1:10">
       <c r="A24" s="19"/>
@@ -1910,16 +1912,16 @@
       <c r="J25" s="19"/>
     </row>
     <row r="26" spans="1:10">
-      <c r="A26" s="29">
+      <c r="A26" s="101">
         <v>2619</v>
       </c>
-      <c r="B26" s="30">
+      <c r="B26" s="29">
         <v>2.6190000000000001E-2</v>
       </c>
-      <c r="C26" s="30">
+      <c r="C26" s="29">
         <v>0.14954605150459657</v>
       </c>
-      <c r="D26" s="30"/>
+      <c r="D26" s="29"/>
       <c r="E26" s="3"/>
       <c r="F26" s="19"/>
       <c r="G26" s="19"/>
@@ -1928,16 +1930,16 @@
       <c r="J26" s="19"/>
     </row>
     <row r="27" spans="1:10">
-      <c r="A27" s="31" t="s">
+      <c r="A27" s="30" t="s">
         <v>19</v>
       </c>
-      <c r="B27" s="31" t="s">
+      <c r="B27" s="30" t="s">
         <v>20</v>
       </c>
-      <c r="C27" s="31" t="s">
+      <c r="C27" s="30" t="s">
         <v>21</v>
       </c>
-      <c r="D27" s="31"/>
+      <c r="D27" s="30"/>
       <c r="E27" s="3"/>
       <c r="F27" s="19"/>
       <c r="G27" s="19"/>
@@ -1958,14 +1960,14 @@
       <c r="J28" s="19"/>
     </row>
     <row r="29" spans="1:10" ht="20.100000000000001" customHeight="1">
-      <c r="A29" s="54">
+      <c r="A29" s="53">
         <v>27</v>
       </c>
-      <c r="B29" s="54">
+      <c r="B29" s="53">
         <v>3</v>
       </c>
-      <c r="C29" s="55"/>
-      <c r="D29" s="55"/>
+      <c r="C29" s="54"/>
+      <c r="D29" s="54"/>
       <c r="E29" s="3"/>
       <c r="F29" s="19"/>
       <c r="G29" s="19"/>
@@ -1974,14 +1976,14 @@
       <c r="J29" s="19"/>
     </row>
     <row r="30" spans="1:10" ht="20.100000000000001" customHeight="1">
-      <c r="A30" s="56" t="s">
+      <c r="A30" s="55" t="s">
         <v>30</v>
       </c>
-      <c r="B30" s="56" t="s">
+      <c r="B30" s="55" t="s">
         <v>31</v>
       </c>
-      <c r="C30" s="56"/>
-      <c r="D30" s="56"/>
+      <c r="C30" s="55"/>
+      <c r="D30" s="55"/>
       <c r="E30" s="3"/>
       <c r="F30" s="19"/>
       <c r="G30" s="19"/>
@@ -2026,7 +2028,7 @@
       <c r="J33" s="19"/>
     </row>
     <row r="34" spans="1:10" ht="15.6">
-      <c r="A34" s="81" t="s">
+      <c r="A34" s="95" t="s">
         <v>22</v>
       </c>
       <c r="B34" s="26"/>
@@ -2040,7 +2042,7 @@
       <c r="J34" s="19"/>
     </row>
     <row r="35" spans="1:10">
-      <c r="A35" s="81"/>
+      <c r="A35" s="95"/>
       <c r="B35" s="19"/>
       <c r="C35" s="19"/>
       <c r="D35" s="19"/>
@@ -2054,8 +2056,8 @@
     <row r="36" spans="1:10" ht="31.2">
       <c r="A36" s="19"/>
       <c r="B36" s="19"/>
-      <c r="C36" s="53"/>
-      <c r="D36" s="53"/>
+      <c r="C36" s="52"/>
+      <c r="D36" s="52"/>
       <c r="E36" s="3"/>
       <c r="F36" s="19"/>
       <c r="G36" s="19"/>
@@ -2068,10 +2070,10 @@
       <c r="B37" s="27" t="s">
         <v>23</v>
       </c>
-      <c r="C37" s="32">
+      <c r="C37" s="102">
         <v>1340</v>
       </c>
-      <c r="D37" s="32"/>
+      <c r="D37" s="31"/>
       <c r="E37" s="3"/>
       <c r="F37" s="19"/>
       <c r="G37" s="19"/>
@@ -2084,10 +2086,10 @@
       <c r="B38" s="27" t="s">
         <v>24</v>
       </c>
-      <c r="C38" s="33">
+      <c r="C38" s="103">
         <v>1279</v>
       </c>
-      <c r="D38" s="33"/>
+      <c r="D38" s="32"/>
       <c r="E38" s="3"/>
       <c r="F38" s="19"/>
       <c r="G38" s="19"/>
@@ -2120,7 +2122,7 @@
       <c r="J40" s="19"/>
     </row>
     <row r="41" spans="1:10" ht="15.6" customHeight="1">
-      <c r="A41" s="81" t="s">
+      <c r="A41" s="95" t="s">
         <v>33</v>
       </c>
       <c r="B41" s="19"/>
@@ -2134,7 +2136,7 @@
       <c r="J41" s="19"/>
     </row>
     <row r="42" spans="1:10" ht="14.4" customHeight="1">
-      <c r="A42" s="81"/>
+      <c r="A42" s="95"/>
       <c r="B42" s="19"/>
       <c r="C42" s="19"/>
       <c r="D42" s="19"/>
@@ -2159,11 +2161,11 @@
     </row>
     <row r="44" spans="1:10" ht="18">
       <c r="A44" s="19"/>
-      <c r="B44" s="77" t="s">
+      <c r="B44" s="76" t="s">
         <v>34</v>
       </c>
-      <c r="C44" s="78">
-        <v>972</v>
+      <c r="C44" s="104">
+        <v>1972</v>
       </c>
       <c r="D44" s="19"/>
       <c r="E44" s="3"/>
@@ -2175,11 +2177,11 @@
     </row>
     <row r="45" spans="1:10" ht="18">
       <c r="A45" s="19"/>
-      <c r="B45" s="79" t="s">
+      <c r="B45" s="77" t="s">
         <v>35</v>
       </c>
-      <c r="C45" s="78">
-        <v>972</v>
+      <c r="C45" s="104">
+        <v>1972</v>
       </c>
       <c r="D45" s="19"/>
       <c r="E45" s="3"/>
@@ -2250,7 +2252,7 @@
       <c r="J50" s="3"/>
     </row>
     <row r="51" spans="1:10">
-      <c r="A51" s="58" t="s">
+      <c r="A51" s="57" t="s">
         <v>25</v>
       </c>
       <c r="B51" s="9"/>
@@ -2474,7 +2476,7 @@
       <c r="D69" s="7"/>
       <c r="E69" s="7"/>
       <c r="F69" s="7"/>
-      <c r="G69" s="59"/>
+      <c r="G69" s="58"/>
       <c r="H69" s="7"/>
       <c r="I69" s="7"/>
       <c r="J69" s="7"/>
@@ -2486,7 +2488,7 @@
       <c r="D70" s="7"/>
       <c r="E70" s="7"/>
       <c r="F70" s="7"/>
-      <c r="G70" s="64"/>
+      <c r="G70" s="63"/>
       <c r="H70" s="7"/>
       <c r="I70" s="7"/>
       <c r="J70" s="7"/>
@@ -2498,7 +2500,7 @@
       <c r="D71" s="7"/>
       <c r="E71" s="7"/>
       <c r="F71" s="7"/>
-      <c r="G71" s="64"/>
+      <c r="G71" s="63"/>
       <c r="H71" s="7"/>
       <c r="I71" s="7"/>
       <c r="J71" s="7"/>
@@ -2511,59 +2513,59 @@
       <c r="E72" s="7"/>
       <c r="F72" s="7"/>
       <c r="I72" s="7"/>
-      <c r="J72" s="76" t="s">
+      <c r="J72" s="75" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="73" spans="1:10" ht="21">
-      <c r="A73" s="89" t="s">
+      <c r="A73" s="91" t="s">
         <v>10</v>
       </c>
-      <c r="B73" s="91" t="s">
+      <c r="B73" s="93" t="s">
         <v>4</v>
       </c>
-      <c r="C73" s="91"/>
-      <c r="D73" s="91"/>
-      <c r="E73" s="91"/>
-      <c r="F73" s="91"/>
-      <c r="G73" s="91"/>
-      <c r="H73" s="49" t="s">
+      <c r="C73" s="93"/>
+      <c r="D73" s="93"/>
+      <c r="E73" s="93"/>
+      <c r="F73" s="93"/>
+      <c r="G73" s="93"/>
+      <c r="H73" s="48" t="s">
         <v>11</v>
       </c>
-      <c r="I73" s="50"/>
-      <c r="J73" s="51">
+      <c r="I73" s="49"/>
+      <c r="J73" s="50">
         <v>2665</v>
       </c>
     </row>
     <row r="74" spans="1:10" ht="21">
-      <c r="A74" s="90"/>
-      <c r="B74" s="92"/>
-      <c r="C74" s="92"/>
-      <c r="D74" s="92"/>
-      <c r="E74" s="92"/>
-      <c r="F74" s="92"/>
-      <c r="G74" s="92"/>
-      <c r="H74" s="49" t="s">
+      <c r="A74" s="92"/>
+      <c r="B74" s="94"/>
+      <c r="C74" s="94"/>
+      <c r="D74" s="94"/>
+      <c r="E74" s="94"/>
+      <c r="F74" s="94"/>
+      <c r="G74" s="94"/>
+      <c r="H74" s="48" t="s">
         <v>12</v>
       </c>
-      <c r="I74" s="50"/>
-      <c r="J74" s="52">
+      <c r="I74" s="49"/>
+      <c r="J74" s="51">
         <v>42901</v>
       </c>
     </row>
     <row r="75" spans="1:10" ht="21">
-      <c r="A75" s="90"/>
-      <c r="B75" s="92"/>
-      <c r="C75" s="92"/>
-      <c r="D75" s="92"/>
-      <c r="E75" s="92"/>
-      <c r="F75" s="92"/>
-      <c r="G75" s="92"/>
-      <c r="H75" s="49" t="s">
+      <c r="A75" s="92"/>
+      <c r="B75" s="94"/>
+      <c r="C75" s="94"/>
+      <c r="D75" s="94"/>
+      <c r="E75" s="94"/>
+      <c r="F75" s="94"/>
+      <c r="G75" s="94"/>
+      <c r="H75" s="48" t="s">
         <v>5</v>
       </c>
-      <c r="I75" s="50"/>
-      <c r="J75" s="52">
+      <c r="I75" s="49"/>
+      <c r="J75" s="51">
         <v>42901</v>
       </c>
     </row>
@@ -2618,563 +2620,558 @@
       <c r="J79" s="8"/>
     </row>
     <row r="80" spans="1:10" ht="23.4">
-      <c r="A80" s="95" t="s">
+      <c r="A80" s="89" t="s">
         <v>0</v>
       </c>
-      <c r="B80" s="95"/>
-      <c r="C80" s="95"/>
-      <c r="D80" s="95"/>
-      <c r="E80" s="96"/>
-      <c r="F80" s="66" t="s">
+      <c r="B80" s="89"/>
+      <c r="C80" s="89"/>
+      <c r="D80" s="89"/>
+      <c r="E80" s="90"/>
+      <c r="F80" s="65" t="s">
         <v>19</v>
       </c>
-      <c r="G80" s="67" t="s">
+      <c r="G80" s="66" t="s">
         <v>1</v>
       </c>
-      <c r="H80" s="67" t="s">
+      <c r="H80" s="66" t="s">
         <v>2</v>
       </c>
-      <c r="I80" s="66" t="s">
+      <c r="I80" s="65" t="s">
         <v>3</v>
       </c>
-      <c r="J80" s="65"/>
+      <c r="J80" s="64"/>
     </row>
     <row r="81" spans="1:10">
-      <c r="A81" s="62"/>
-      <c r="B81" s="62"/>
-      <c r="C81" s="62"/>
-      <c r="D81" s="62"/>
-      <c r="E81" s="62"/>
-      <c r="F81" s="62"/>
-      <c r="G81" s="62"/>
-      <c r="H81" s="62"/>
-      <c r="I81" s="62"/>
-      <c r="J81" s="63"/>
+      <c r="A81" s="61"/>
+      <c r="B81" s="61"/>
+      <c r="C81" s="61"/>
+      <c r="D81" s="61"/>
+      <c r="E81" s="61"/>
+      <c r="F81" s="61"/>
+      <c r="G81" s="61"/>
+      <c r="H81" s="61"/>
+      <c r="I81" s="61"/>
+      <c r="J81" s="62"/>
     </row>
     <row r="82" spans="1:10" ht="50.1" customHeight="1">
-      <c r="A82" s="97"/>
-      <c r="B82" s="98"/>
-      <c r="C82" s="98"/>
-      <c r="D82" s="98"/>
-      <c r="E82" s="98"/>
-      <c r="F82" s="68"/>
-      <c r="G82" s="68"/>
-      <c r="H82" s="68"/>
-      <c r="I82" s="69" t="s">
+      <c r="A82" s="87"/>
+      <c r="B82" s="88"/>
+      <c r="C82" s="88"/>
+      <c r="D82" s="88"/>
+      <c r="E82" s="88"/>
+      <c r="F82" s="67"/>
+      <c r="G82" s="67"/>
+      <c r="H82" s="67"/>
+      <c r="I82" s="68" t="s">
         <v>32</v>
       </c>
       <c r="J82" s="3"/>
     </row>
     <row r="83" spans="1:10" ht="50.1" customHeight="1">
-      <c r="A83" s="87"/>
-      <c r="B83" s="88"/>
-      <c r="C83" s="88"/>
-      <c r="D83" s="88"/>
-      <c r="E83" s="88"/>
-      <c r="F83" s="61"/>
-      <c r="G83" s="61"/>
-      <c r="H83" s="61"/>
-      <c r="I83" s="70" t="s">
+      <c r="A83" s="78"/>
+      <c r="B83" s="79"/>
+      <c r="C83" s="79"/>
+      <c r="D83" s="79"/>
+      <c r="E83" s="79"/>
+      <c r="F83" s="60"/>
+      <c r="G83" s="60"/>
+      <c r="H83" s="60"/>
+      <c r="I83" s="69" t="s">
         <v>32</v>
       </c>
       <c r="J83" s="3"/>
     </row>
     <row r="84" spans="1:10" ht="50.1" customHeight="1">
-      <c r="A84" s="85"/>
-      <c r="B84" s="86"/>
-      <c r="C84" s="86"/>
-      <c r="D84" s="86"/>
-      <c r="E84" s="86"/>
-      <c r="F84" s="60"/>
-      <c r="G84" s="60"/>
-      <c r="H84" s="60"/>
-      <c r="I84" s="71" t="s">
+      <c r="A84" s="80"/>
+      <c r="B84" s="81"/>
+      <c r="C84" s="81"/>
+      <c r="D84" s="81"/>
+      <c r="E84" s="81"/>
+      <c r="F84" s="59"/>
+      <c r="G84" s="59"/>
+      <c r="H84" s="59"/>
+      <c r="I84" s="70" t="s">
         <v>32</v>
       </c>
       <c r="J84" s="3"/>
     </row>
     <row r="85" spans="1:10" ht="50.1" customHeight="1">
-      <c r="A85" s="87"/>
-      <c r="B85" s="88"/>
-      <c r="C85" s="88"/>
-      <c r="D85" s="88"/>
-      <c r="E85" s="88"/>
-      <c r="F85" s="61"/>
-      <c r="G85" s="61"/>
-      <c r="H85" s="61"/>
-      <c r="I85" s="70" t="s">
+      <c r="A85" s="78"/>
+      <c r="B85" s="79"/>
+      <c r="C85" s="79"/>
+      <c r="D85" s="79"/>
+      <c r="E85" s="79"/>
+      <c r="F85" s="60"/>
+      <c r="G85" s="60"/>
+      <c r="H85" s="60"/>
+      <c r="I85" s="69" t="s">
         <v>32</v>
       </c>
       <c r="J85" s="3"/>
     </row>
     <row r="86" spans="1:10" ht="50.1" customHeight="1">
-      <c r="A86" s="85"/>
-      <c r="B86" s="86"/>
-      <c r="C86" s="86"/>
-      <c r="D86" s="86"/>
-      <c r="E86" s="86"/>
-      <c r="F86" s="60"/>
-      <c r="G86" s="60"/>
-      <c r="H86" s="60"/>
-      <c r="I86" s="71" t="s">
+      <c r="A86" s="80"/>
+      <c r="B86" s="81"/>
+      <c r="C86" s="81"/>
+      <c r="D86" s="81"/>
+      <c r="E86" s="81"/>
+      <c r="F86" s="59"/>
+      <c r="G86" s="59"/>
+      <c r="H86" s="59"/>
+      <c r="I86" s="70" t="s">
         <v>32</v>
       </c>
       <c r="J86" s="3"/>
     </row>
     <row r="87" spans="1:10" ht="50.1" customHeight="1">
-      <c r="A87" s="87"/>
-      <c r="B87" s="88"/>
-      <c r="C87" s="88"/>
-      <c r="D87" s="88"/>
-      <c r="E87" s="88"/>
-      <c r="F87" s="61"/>
-      <c r="G87" s="61"/>
-      <c r="H87" s="61"/>
-      <c r="I87" s="70" t="s">
+      <c r="A87" s="78"/>
+      <c r="B87" s="79"/>
+      <c r="C87" s="79"/>
+      <c r="D87" s="79"/>
+      <c r="E87" s="79"/>
+      <c r="F87" s="60"/>
+      <c r="G87" s="60"/>
+      <c r="H87" s="60"/>
+      <c r="I87" s="69" t="s">
         <v>32</v>
       </c>
       <c r="J87" s="3"/>
     </row>
     <row r="88" spans="1:10" ht="50.1" customHeight="1">
-      <c r="A88" s="85"/>
-      <c r="B88" s="86"/>
-      <c r="C88" s="86"/>
-      <c r="D88" s="86"/>
-      <c r="E88" s="86"/>
-      <c r="F88" s="60"/>
-      <c r="G88" s="60"/>
-      <c r="H88" s="60"/>
-      <c r="I88" s="71" t="s">
+      <c r="A88" s="80"/>
+      <c r="B88" s="81"/>
+      <c r="C88" s="81"/>
+      <c r="D88" s="81"/>
+      <c r="E88" s="81"/>
+      <c r="F88" s="59"/>
+      <c r="G88" s="59"/>
+      <c r="H88" s="59"/>
+      <c r="I88" s="70" t="s">
         <v>32</v>
       </c>
       <c r="J88" s="3"/>
     </row>
     <row r="89" spans="1:10" ht="50.1" customHeight="1">
-      <c r="A89" s="87"/>
-      <c r="B89" s="88"/>
-      <c r="C89" s="88"/>
-      <c r="D89" s="88"/>
-      <c r="E89" s="88"/>
-      <c r="F89" s="61"/>
-      <c r="G89" s="61"/>
-      <c r="H89" s="61"/>
-      <c r="I89" s="70" t="s">
+      <c r="A89" s="78"/>
+      <c r="B89" s="79"/>
+      <c r="C89" s="79"/>
+      <c r="D89" s="79"/>
+      <c r="E89" s="79"/>
+      <c r="F89" s="60"/>
+      <c r="G89" s="60"/>
+      <c r="H89" s="60"/>
+      <c r="I89" s="69" t="s">
         <v>32</v>
       </c>
       <c r="J89" s="3"/>
     </row>
     <row r="90" spans="1:10" ht="50.1" customHeight="1">
-      <c r="A90" s="85"/>
-      <c r="B90" s="86"/>
-      <c r="C90" s="86"/>
-      <c r="D90" s="86"/>
-      <c r="E90" s="86"/>
-      <c r="F90" s="60"/>
-      <c r="G90" s="60"/>
-      <c r="H90" s="60"/>
-      <c r="I90" s="71" t="s">
+      <c r="A90" s="80"/>
+      <c r="B90" s="81"/>
+      <c r="C90" s="81"/>
+      <c r="D90" s="81"/>
+      <c r="E90" s="81"/>
+      <c r="F90" s="59"/>
+      <c r="G90" s="59"/>
+      <c r="H90" s="59"/>
+      <c r="I90" s="70" t="s">
         <v>32</v>
       </c>
       <c r="J90" s="3"/>
     </row>
     <row r="91" spans="1:10" ht="50.1" customHeight="1">
-      <c r="A91" s="87"/>
-      <c r="B91" s="88"/>
-      <c r="C91" s="88"/>
-      <c r="D91" s="88"/>
-      <c r="E91" s="88"/>
-      <c r="F91" s="61"/>
-      <c r="G91" s="61"/>
-      <c r="H91" s="61"/>
-      <c r="I91" s="70" t="s">
+      <c r="A91" s="78"/>
+      <c r="B91" s="79"/>
+      <c r="C91" s="79"/>
+      <c r="D91" s="79"/>
+      <c r="E91" s="79"/>
+      <c r="F91" s="60"/>
+      <c r="G91" s="60"/>
+      <c r="H91" s="60"/>
+      <c r="I91" s="69" t="s">
         <v>32</v>
       </c>
       <c r="J91" s="3"/>
     </row>
     <row r="92" spans="1:10" ht="50.1" customHeight="1">
-      <c r="A92" s="85"/>
-      <c r="B92" s="86"/>
-      <c r="C92" s="86"/>
-      <c r="D92" s="86"/>
-      <c r="E92" s="86"/>
-      <c r="F92" s="60"/>
-      <c r="G92" s="60"/>
-      <c r="H92" s="60"/>
-      <c r="I92" s="72" t="s">
+      <c r="A92" s="80"/>
+      <c r="B92" s="81"/>
+      <c r="C92" s="81"/>
+      <c r="D92" s="81"/>
+      <c r="E92" s="81"/>
+      <c r="F92" s="59"/>
+      <c r="G92" s="59"/>
+      <c r="H92" s="59"/>
+      <c r="I92" s="71" t="s">
         <v>32</v>
       </c>
       <c r="J92" s="3"/>
     </row>
     <row r="93" spans="1:10" ht="50.1" customHeight="1">
-      <c r="A93" s="87"/>
-      <c r="B93" s="88"/>
-      <c r="C93" s="88"/>
-      <c r="D93" s="88"/>
-      <c r="E93" s="88"/>
-      <c r="F93" s="61"/>
-      <c r="G93" s="61"/>
-      <c r="H93" s="61"/>
-      <c r="I93" s="73" t="s">
+      <c r="A93" s="78"/>
+      <c r="B93" s="79"/>
+      <c r="C93" s="79"/>
+      <c r="D93" s="79"/>
+      <c r="E93" s="79"/>
+      <c r="F93" s="60"/>
+      <c r="G93" s="60"/>
+      <c r="H93" s="60"/>
+      <c r="I93" s="72" t="s">
         <v>32</v>
       </c>
       <c r="J93" s="3"/>
     </row>
     <row r="94" spans="1:10" ht="50.1" customHeight="1">
-      <c r="A94" s="85"/>
-      <c r="B94" s="86"/>
-      <c r="C94" s="86"/>
-      <c r="D94" s="86"/>
-      <c r="E94" s="86"/>
-      <c r="F94" s="60"/>
-      <c r="G94" s="60"/>
-      <c r="H94" s="60"/>
-      <c r="I94" s="71" t="s">
+      <c r="A94" s="80"/>
+      <c r="B94" s="81"/>
+      <c r="C94" s="81"/>
+      <c r="D94" s="81"/>
+      <c r="E94" s="81"/>
+      <c r="F94" s="59"/>
+      <c r="G94" s="59"/>
+      <c r="H94" s="59"/>
+      <c r="I94" s="70" t="s">
         <v>32</v>
       </c>
       <c r="J94" s="3"/>
     </row>
     <row r="95" spans="1:10" ht="50.1" customHeight="1">
-      <c r="A95" s="99"/>
-      <c r="B95" s="100"/>
-      <c r="C95" s="100"/>
-      <c r="D95" s="100"/>
-      <c r="E95" s="101"/>
-      <c r="F95" s="61"/>
-      <c r="G95" s="61"/>
-      <c r="H95" s="61"/>
-      <c r="I95" s="70" t="s">
+      <c r="A95" s="84"/>
+      <c r="B95" s="85"/>
+      <c r="C95" s="85"/>
+      <c r="D95" s="85"/>
+      <c r="E95" s="86"/>
+      <c r="F95" s="60"/>
+      <c r="G95" s="60"/>
+      <c r="H95" s="60"/>
+      <c r="I95" s="69" t="s">
         <v>32</v>
       </c>
       <c r="J95" s="3"/>
     </row>
     <row r="96" spans="1:10" ht="50.1" customHeight="1">
-      <c r="A96" s="85"/>
-      <c r="B96" s="86"/>
-      <c r="C96" s="86"/>
-      <c r="D96" s="86"/>
-      <c r="E96" s="86"/>
-      <c r="F96" s="60"/>
-      <c r="G96" s="60"/>
-      <c r="H96" s="60"/>
-      <c r="I96" s="71" t="s">
+      <c r="A96" s="80"/>
+      <c r="B96" s="81"/>
+      <c r="C96" s="81"/>
+      <c r="D96" s="81"/>
+      <c r="E96" s="81"/>
+      <c r="F96" s="59"/>
+      <c r="G96" s="59"/>
+      <c r="H96" s="59"/>
+      <c r="I96" s="70" t="s">
         <v>32</v>
       </c>
       <c r="J96" s="3"/>
     </row>
     <row r="97" spans="1:10" ht="50.1" customHeight="1">
-      <c r="A97" s="87"/>
-      <c r="B97" s="88"/>
-      <c r="C97" s="88"/>
-      <c r="D97" s="88"/>
-      <c r="E97" s="88"/>
-      <c r="F97" s="61"/>
-      <c r="G97" s="61"/>
-      <c r="H97" s="61"/>
-      <c r="I97" s="70" t="s">
+      <c r="A97" s="78"/>
+      <c r="B97" s="79"/>
+      <c r="C97" s="79"/>
+      <c r="D97" s="79"/>
+      <c r="E97" s="79"/>
+      <c r="F97" s="60"/>
+      <c r="G97" s="60"/>
+      <c r="H97" s="60"/>
+      <c r="I97" s="69" t="s">
         <v>32</v>
       </c>
       <c r="J97" s="3"/>
     </row>
     <row r="98" spans="1:10" ht="50.1" customHeight="1">
-      <c r="A98" s="85"/>
-      <c r="B98" s="86"/>
-      <c r="C98" s="86"/>
-      <c r="D98" s="86"/>
-      <c r="E98" s="86"/>
-      <c r="F98" s="60"/>
-      <c r="G98" s="60"/>
-      <c r="H98" s="60"/>
-      <c r="I98" s="72" t="s">
+      <c r="A98" s="80"/>
+      <c r="B98" s="81"/>
+      <c r="C98" s="81"/>
+      <c r="D98" s="81"/>
+      <c r="E98" s="81"/>
+      <c r="F98" s="59"/>
+      <c r="G98" s="59"/>
+      <c r="H98" s="59"/>
+      <c r="I98" s="71" t="s">
         <v>32</v>
       </c>
       <c r="J98" s="3"/>
     </row>
     <row r="99" spans="1:10" ht="50.1" customHeight="1">
-      <c r="A99" s="93"/>
-      <c r="B99" s="94"/>
-      <c r="C99" s="94"/>
-      <c r="D99" s="94"/>
-      <c r="E99" s="94"/>
-      <c r="F99" s="74"/>
-      <c r="G99" s="74"/>
-      <c r="H99" s="74"/>
-      <c r="I99" s="75" t="s">
+      <c r="A99" s="82"/>
+      <c r="B99" s="83"/>
+      <c r="C99" s="83"/>
+      <c r="D99" s="83"/>
+      <c r="E99" s="83"/>
+      <c r="F99" s="73"/>
+      <c r="G99" s="73"/>
+      <c r="H99" s="73"/>
+      <c r="I99" s="74" t="s">
         <v>32</v>
       </c>
       <c r="J99" s="3"/>
     </row>
     <row r="100" spans="1:10" ht="50.1" customHeight="1">
-      <c r="A100" s="97"/>
-      <c r="B100" s="98"/>
-      <c r="C100" s="98"/>
-      <c r="D100" s="98"/>
-      <c r="E100" s="98"/>
-      <c r="F100" s="68"/>
-      <c r="G100" s="68"/>
-      <c r="H100" s="68"/>
-      <c r="I100" s="69" t="s">
+      <c r="A100" s="87"/>
+      <c r="B100" s="88"/>
+      <c r="C100" s="88"/>
+      <c r="D100" s="88"/>
+      <c r="E100" s="88"/>
+      <c r="F100" s="67"/>
+      <c r="G100" s="67"/>
+      <c r="H100" s="67"/>
+      <c r="I100" s="68" t="s">
         <v>32</v>
       </c>
       <c r="J100" s="3"/>
     </row>
     <row r="101" spans="1:10" ht="50.1" customHeight="1">
-      <c r="A101" s="87"/>
-      <c r="B101" s="88"/>
-      <c r="C101" s="88"/>
-      <c r="D101" s="88"/>
-      <c r="E101" s="88"/>
-      <c r="F101" s="61"/>
-      <c r="G101" s="61"/>
-      <c r="H101" s="61"/>
-      <c r="I101" s="70" t="s">
+      <c r="A101" s="78"/>
+      <c r="B101" s="79"/>
+      <c r="C101" s="79"/>
+      <c r="D101" s="79"/>
+      <c r="E101" s="79"/>
+      <c r="F101" s="60"/>
+      <c r="G101" s="60"/>
+      <c r="H101" s="60"/>
+      <c r="I101" s="69" t="s">
         <v>32</v>
       </c>
       <c r="J101" s="3"/>
     </row>
     <row r="102" spans="1:10" ht="50.1" customHeight="1">
-      <c r="A102" s="85"/>
-      <c r="B102" s="86"/>
-      <c r="C102" s="86"/>
-      <c r="D102" s="86"/>
-      <c r="E102" s="86"/>
-      <c r="F102" s="60"/>
-      <c r="G102" s="60"/>
-      <c r="H102" s="60"/>
-      <c r="I102" s="71" t="s">
+      <c r="A102" s="80"/>
+      <c r="B102" s="81"/>
+      <c r="C102" s="81"/>
+      <c r="D102" s="81"/>
+      <c r="E102" s="81"/>
+      <c r="F102" s="59"/>
+      <c r="G102" s="59"/>
+      <c r="H102" s="59"/>
+      <c r="I102" s="70" t="s">
         <v>32</v>
       </c>
       <c r="J102" s="3"/>
     </row>
     <row r="103" spans="1:10" ht="50.1" customHeight="1">
-      <c r="A103" s="87"/>
-      <c r="B103" s="88"/>
-      <c r="C103" s="88"/>
-      <c r="D103" s="88"/>
-      <c r="E103" s="88"/>
-      <c r="F103" s="61"/>
-      <c r="G103" s="61"/>
-      <c r="H103" s="61"/>
-      <c r="I103" s="70" t="s">
+      <c r="A103" s="78"/>
+      <c r="B103" s="79"/>
+      <c r="C103" s="79"/>
+      <c r="D103" s="79"/>
+      <c r="E103" s="79"/>
+      <c r="F103" s="60"/>
+      <c r="G103" s="60"/>
+      <c r="H103" s="60"/>
+      <c r="I103" s="69" t="s">
         <v>32</v>
       </c>
       <c r="J103" s="3"/>
     </row>
     <row r="104" spans="1:10" ht="50.1" customHeight="1">
-      <c r="A104" s="85"/>
-      <c r="B104" s="86"/>
-      <c r="C104" s="86"/>
-      <c r="D104" s="86"/>
-      <c r="E104" s="86"/>
-      <c r="F104" s="60"/>
-      <c r="G104" s="60"/>
-      <c r="H104" s="60"/>
-      <c r="I104" s="71" t="s">
+      <c r="A104" s="80"/>
+      <c r="B104" s="81"/>
+      <c r="C104" s="81"/>
+      <c r="D104" s="81"/>
+      <c r="E104" s="81"/>
+      <c r="F104" s="59"/>
+      <c r="G104" s="59"/>
+      <c r="H104" s="59"/>
+      <c r="I104" s="70" t="s">
         <v>32</v>
       </c>
       <c r="J104" s="3"/>
     </row>
     <row r="105" spans="1:10" ht="50.1" customHeight="1">
-      <c r="A105" s="87"/>
-      <c r="B105" s="88"/>
-      <c r="C105" s="88"/>
-      <c r="D105" s="88"/>
-      <c r="E105" s="88"/>
-      <c r="F105" s="61"/>
-      <c r="G105" s="61"/>
-      <c r="H105" s="61"/>
-      <c r="I105" s="70" t="s">
+      <c r="A105" s="78"/>
+      <c r="B105" s="79"/>
+      <c r="C105" s="79"/>
+      <c r="D105" s="79"/>
+      <c r="E105" s="79"/>
+      <c r="F105" s="60"/>
+      <c r="G105" s="60"/>
+      <c r="H105" s="60"/>
+      <c r="I105" s="69" t="s">
         <v>32</v>
       </c>
       <c r="J105" s="3"/>
     </row>
     <row r="106" spans="1:10" ht="50.1" customHeight="1">
-      <c r="A106" s="85"/>
-      <c r="B106" s="86"/>
-      <c r="C106" s="86"/>
-      <c r="D106" s="86"/>
-      <c r="E106" s="86"/>
-      <c r="F106" s="60"/>
-      <c r="G106" s="60"/>
-      <c r="H106" s="60"/>
-      <c r="I106" s="71" t="s">
+      <c r="A106" s="80"/>
+      <c r="B106" s="81"/>
+      <c r="C106" s="81"/>
+      <c r="D106" s="81"/>
+      <c r="E106" s="81"/>
+      <c r="F106" s="59"/>
+      <c r="G106" s="59"/>
+      <c r="H106" s="59"/>
+      <c r="I106" s="70" t="s">
         <v>32</v>
       </c>
       <c r="J106" s="3"/>
     </row>
     <row r="107" spans="1:10" ht="50.1" customHeight="1">
-      <c r="A107" s="87"/>
-      <c r="B107" s="88"/>
-      <c r="C107" s="88"/>
-      <c r="D107" s="88"/>
-      <c r="E107" s="88"/>
-      <c r="F107" s="61"/>
-      <c r="G107" s="61"/>
-      <c r="H107" s="61"/>
-      <c r="I107" s="70" t="s">
+      <c r="A107" s="78"/>
+      <c r="B107" s="79"/>
+      <c r="C107" s="79"/>
+      <c r="D107" s="79"/>
+      <c r="E107" s="79"/>
+      <c r="F107" s="60"/>
+      <c r="G107" s="60"/>
+      <c r="H107" s="60"/>
+      <c r="I107" s="69" t="s">
         <v>32</v>
       </c>
       <c r="J107" s="3"/>
     </row>
     <row r="108" spans="1:10" ht="50.1" customHeight="1">
-      <c r="A108" s="85"/>
-      <c r="B108" s="86"/>
-      <c r="C108" s="86"/>
-      <c r="D108" s="86"/>
-      <c r="E108" s="86"/>
-      <c r="F108" s="60"/>
-      <c r="G108" s="60"/>
-      <c r="H108" s="60"/>
-      <c r="I108" s="71" t="s">
+      <c r="A108" s="80"/>
+      <c r="B108" s="81"/>
+      <c r="C108" s="81"/>
+      <c r="D108" s="81"/>
+      <c r="E108" s="81"/>
+      <c r="F108" s="59"/>
+      <c r="G108" s="59"/>
+      <c r="H108" s="59"/>
+      <c r="I108" s="70" t="s">
         <v>32</v>
       </c>
       <c r="J108" s="3"/>
     </row>
     <row r="109" spans="1:10" ht="50.1" customHeight="1">
-      <c r="A109" s="87"/>
-      <c r="B109" s="88"/>
-      <c r="C109" s="88"/>
-      <c r="D109" s="88"/>
-      <c r="E109" s="88"/>
-      <c r="F109" s="61"/>
-      <c r="G109" s="61"/>
-      <c r="H109" s="61"/>
-      <c r="I109" s="70" t="s">
+      <c r="A109" s="78"/>
+      <c r="B109" s="79"/>
+      <c r="C109" s="79"/>
+      <c r="D109" s="79"/>
+      <c r="E109" s="79"/>
+      <c r="F109" s="60"/>
+      <c r="G109" s="60"/>
+      <c r="H109" s="60"/>
+      <c r="I109" s="69" t="s">
         <v>32</v>
       </c>
       <c r="J109" s="3"/>
     </row>
     <row r="110" spans="1:10" ht="50.1" customHeight="1">
-      <c r="A110" s="85"/>
-      <c r="B110" s="86"/>
-      <c r="C110" s="86"/>
-      <c r="D110" s="86"/>
-      <c r="E110" s="86"/>
-      <c r="F110" s="60"/>
-      <c r="G110" s="60"/>
-      <c r="H110" s="60"/>
-      <c r="I110" s="72" t="s">
+      <c r="A110" s="80"/>
+      <c r="B110" s="81"/>
+      <c r="C110" s="81"/>
+      <c r="D110" s="81"/>
+      <c r="E110" s="81"/>
+      <c r="F110" s="59"/>
+      <c r="G110" s="59"/>
+      <c r="H110" s="59"/>
+      <c r="I110" s="71" t="s">
         <v>32</v>
       </c>
       <c r="J110" s="3"/>
     </row>
     <row r="111" spans="1:10" ht="50.1" customHeight="1">
-      <c r="A111" s="87"/>
-      <c r="B111" s="88"/>
-      <c r="C111" s="88"/>
-      <c r="D111" s="88"/>
-      <c r="E111" s="88"/>
-      <c r="F111" s="61"/>
-      <c r="G111" s="61"/>
-      <c r="H111" s="61"/>
-      <c r="I111" s="73" t="s">
+      <c r="A111" s="78"/>
+      <c r="B111" s="79"/>
+      <c r="C111" s="79"/>
+      <c r="D111" s="79"/>
+      <c r="E111" s="79"/>
+      <c r="F111" s="60"/>
+      <c r="G111" s="60"/>
+      <c r="H111" s="60"/>
+      <c r="I111" s="72" t="s">
         <v>32</v>
       </c>
       <c r="J111" s="3"/>
     </row>
     <row r="112" spans="1:10" ht="50.1" customHeight="1">
-      <c r="A112" s="85"/>
-      <c r="B112" s="86"/>
-      <c r="C112" s="86"/>
-      <c r="D112" s="86"/>
-      <c r="E112" s="86"/>
-      <c r="F112" s="60"/>
-      <c r="G112" s="60"/>
-      <c r="H112" s="60"/>
-      <c r="I112" s="71" t="s">
+      <c r="A112" s="80"/>
+      <c r="B112" s="81"/>
+      <c r="C112" s="81"/>
+      <c r="D112" s="81"/>
+      <c r="E112" s="81"/>
+      <c r="F112" s="59"/>
+      <c r="G112" s="59"/>
+      <c r="H112" s="59"/>
+      <c r="I112" s="70" t="s">
         <v>32</v>
       </c>
       <c r="J112" s="3"/>
     </row>
     <row r="113" spans="1:10" ht="50.1" customHeight="1">
-      <c r="A113" s="99"/>
-      <c r="B113" s="100"/>
-      <c r="C113" s="100"/>
-      <c r="D113" s="100"/>
-      <c r="E113" s="101"/>
-      <c r="F113" s="61"/>
-      <c r="G113" s="61"/>
-      <c r="H113" s="61"/>
-      <c r="I113" s="70" t="s">
+      <c r="A113" s="84"/>
+      <c r="B113" s="85"/>
+      <c r="C113" s="85"/>
+      <c r="D113" s="85"/>
+      <c r="E113" s="86"/>
+      <c r="F113" s="60"/>
+      <c r="G113" s="60"/>
+      <c r="H113" s="60"/>
+      <c r="I113" s="69" t="s">
         <v>32</v>
       </c>
       <c r="J113" s="3"/>
     </row>
     <row r="114" spans="1:10" ht="50.1" customHeight="1">
-      <c r="A114" s="85"/>
-      <c r="B114" s="86"/>
-      <c r="C114" s="86"/>
-      <c r="D114" s="86"/>
-      <c r="E114" s="86"/>
-      <c r="F114" s="60"/>
-      <c r="G114" s="60"/>
-      <c r="H114" s="60"/>
-      <c r="I114" s="71" t="s">
+      <c r="A114" s="80"/>
+      <c r="B114" s="81"/>
+      <c r="C114" s="81"/>
+      <c r="D114" s="81"/>
+      <c r="E114" s="81"/>
+      <c r="F114" s="59"/>
+      <c r="G114" s="59"/>
+      <c r="H114" s="59"/>
+      <c r="I114" s="70" t="s">
         <v>32</v>
       </c>
       <c r="J114" s="3"/>
     </row>
     <row r="115" spans="1:10" ht="50.1" customHeight="1">
-      <c r="A115" s="87"/>
-      <c r="B115" s="88"/>
-      <c r="C115" s="88"/>
-      <c r="D115" s="88"/>
-      <c r="E115" s="88"/>
-      <c r="F115" s="61"/>
-      <c r="G115" s="61"/>
-      <c r="H115" s="61"/>
-      <c r="I115" s="70" t="s">
+      <c r="A115" s="78"/>
+      <c r="B115" s="79"/>
+      <c r="C115" s="79"/>
+      <c r="D115" s="79"/>
+      <c r="E115" s="79"/>
+      <c r="F115" s="60"/>
+      <c r="G115" s="60"/>
+      <c r="H115" s="60"/>
+      <c r="I115" s="69" t="s">
         <v>32</v>
       </c>
       <c r="J115" s="3"/>
     </row>
     <row r="116" spans="1:10" ht="50.1" customHeight="1">
-      <c r="A116" s="85"/>
-      <c r="B116" s="86"/>
-      <c r="C116" s="86"/>
-      <c r="D116" s="86"/>
-      <c r="E116" s="86"/>
-      <c r="F116" s="60"/>
-      <c r="G116" s="60"/>
-      <c r="H116" s="60"/>
-      <c r="I116" s="72" t="s">
+      <c r="A116" s="80"/>
+      <c r="B116" s="81"/>
+      <c r="C116" s="81"/>
+      <c r="D116" s="81"/>
+      <c r="E116" s="81"/>
+      <c r="F116" s="59"/>
+      <c r="G116" s="59"/>
+      <c r="H116" s="59"/>
+      <c r="I116" s="71" t="s">
         <v>32</v>
       </c>
       <c r="J116" s="3"/>
     </row>
     <row r="117" spans="1:10" ht="50.1" customHeight="1">
-      <c r="A117" s="93"/>
-      <c r="B117" s="94"/>
-      <c r="C117" s="94"/>
-      <c r="D117" s="94"/>
-      <c r="E117" s="94"/>
-      <c r="F117" s="74"/>
-      <c r="G117" s="74"/>
-      <c r="H117" s="74"/>
-      <c r="I117" s="75" t="s">
+      <c r="A117" s="82"/>
+      <c r="B117" s="83"/>
+      <c r="C117" s="83"/>
+      <c r="D117" s="83"/>
+      <c r="E117" s="83"/>
+      <c r="F117" s="73"/>
+      <c r="G117" s="73"/>
+      <c r="H117" s="73"/>
+      <c r="I117" s="74" t="s">
         <v>32</v>
       </c>
       <c r="J117" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="47">
-    <mergeCell ref="A115:E115"/>
-    <mergeCell ref="A116:E116"/>
-    <mergeCell ref="A117:E117"/>
-    <mergeCell ref="A110:E110"/>
-    <mergeCell ref="A111:E111"/>
-    <mergeCell ref="A112:E112"/>
-    <mergeCell ref="A113:E113"/>
-    <mergeCell ref="A114:E114"/>
-    <mergeCell ref="A105:E105"/>
-    <mergeCell ref="A106:E106"/>
-    <mergeCell ref="A107:E107"/>
-    <mergeCell ref="A108:E108"/>
-    <mergeCell ref="A109:E109"/>
-    <mergeCell ref="A100:E100"/>
-    <mergeCell ref="A101:E101"/>
-    <mergeCell ref="A102:E102"/>
-    <mergeCell ref="A103:E103"/>
-    <mergeCell ref="A104:E104"/>
+    <mergeCell ref="A7:J7"/>
+    <mergeCell ref="A34:A35"/>
+    <mergeCell ref="A17:B17"/>
+    <mergeCell ref="A18:B18"/>
+    <mergeCell ref="A11:J11"/>
+    <mergeCell ref="A84:E84"/>
+    <mergeCell ref="A85:E85"/>
+    <mergeCell ref="A86:E86"/>
+    <mergeCell ref="A8:A10"/>
+    <mergeCell ref="B8:G10"/>
+    <mergeCell ref="A73:A75"/>
+    <mergeCell ref="B73:G75"/>
+    <mergeCell ref="A41:A42"/>
     <mergeCell ref="A97:E97"/>
     <mergeCell ref="A98:E98"/>
     <mergeCell ref="A99:E99"/>
@@ -3191,19 +3188,24 @@
     <mergeCell ref="A90:E90"/>
     <mergeCell ref="A91:E91"/>
     <mergeCell ref="A95:E95"/>
-    <mergeCell ref="A84:E84"/>
-    <mergeCell ref="A85:E85"/>
-    <mergeCell ref="A86:E86"/>
-    <mergeCell ref="A8:A10"/>
-    <mergeCell ref="B8:G10"/>
-    <mergeCell ref="A73:A75"/>
-    <mergeCell ref="B73:G75"/>
-    <mergeCell ref="A41:A42"/>
-    <mergeCell ref="A7:J7"/>
-    <mergeCell ref="A34:A35"/>
-    <mergeCell ref="A17:B17"/>
-    <mergeCell ref="A18:B18"/>
-    <mergeCell ref="A11:J11"/>
+    <mergeCell ref="A100:E100"/>
+    <mergeCell ref="A101:E101"/>
+    <mergeCell ref="A102:E102"/>
+    <mergeCell ref="A103:E103"/>
+    <mergeCell ref="A104:E104"/>
+    <mergeCell ref="A105:E105"/>
+    <mergeCell ref="A106:E106"/>
+    <mergeCell ref="A107:E107"/>
+    <mergeCell ref="A108:E108"/>
+    <mergeCell ref="A109:E109"/>
+    <mergeCell ref="A115:E115"/>
+    <mergeCell ref="A116:E116"/>
+    <mergeCell ref="A117:E117"/>
+    <mergeCell ref="A110:E110"/>
+    <mergeCell ref="A111:E111"/>
+    <mergeCell ref="A112:E112"/>
+    <mergeCell ref="A113:E113"/>
+    <mergeCell ref="A114:E114"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="57" fitToHeight="0" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>

</xml_diff>